<commit_message>
Cleaned up the repository even further and commented all the code
</commit_message>
<xml_diff>
--- a/transformed_data/cartel_networks/test222.xlsx
+++ b/transformed_data/cartel_networks/test222.xlsx
@@ -451,7 +451,7 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>number_of_cartel_firms</t>
+          <t>number_cartel_firms</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
@@ -1556,7 +1556,7 @@
       <c r="CN5" t="inlineStr"/>
       <c r="CO5" t="inlineStr"/>
       <c r="CP5" t="n">
-        <v>663.8512000000001</v>
+        <v>663.85</v>
       </c>
     </row>
     <row r="6">
@@ -12847,16 +12847,16 @@
       <c r="CK83" t="inlineStr"/>
       <c r="CL83" t="inlineStr"/>
       <c r="CM83" t="n">
-        <v>985.9326</v>
+        <v>985.9299999999999</v>
       </c>
       <c r="CN83" t="n">
-        <v>966.8060999999999</v>
+        <v>966.8099999999999</v>
       </c>
       <c r="CO83" t="n">
-        <v>964.9092999999999</v>
+        <v>964.91</v>
       </c>
       <c r="CP83" t="n">
-        <v>976.1424999999999</v>
+        <v>976.14</v>
       </c>
     </row>
     <row r="84">
@@ -15017,7 +15017,7 @@
       <c r="BG98" t="inlineStr"/>
       <c r="BH98" t="inlineStr"/>
       <c r="BI98" t="n">
-        <v>48.8003</v>
+        <v>48.8</v>
       </c>
       <c r="BJ98" t="inlineStr"/>
       <c r="BK98" t="inlineStr"/>
@@ -15049,16 +15049,16 @@
       <c r="CK98" t="inlineStr"/>
       <c r="CL98" t="inlineStr"/>
       <c r="CM98" t="n">
-        <v>186.4086</v>
+        <v>186.41</v>
       </c>
       <c r="CN98" t="n">
-        <v>196.1324</v>
+        <v>196.13</v>
       </c>
       <c r="CO98" t="n">
-        <v>4.7667</v>
+        <v>4.77</v>
       </c>
       <c r="CP98" t="n">
-        <v>3.5171</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="99">
@@ -17698,7 +17698,7 @@
       <c r="BP116" t="inlineStr"/>
       <c r="BQ116" t="inlineStr"/>
       <c r="BR116" t="n">
-        <v>48.8003</v>
+        <v>48.8</v>
       </c>
       <c r="BS116" t="inlineStr"/>
       <c r="BT116" t="inlineStr"/>
@@ -17721,16 +17721,16 @@
       <c r="CK116" t="inlineStr"/>
       <c r="CL116" t="inlineStr"/>
       <c r="CM116" t="n">
-        <v>186.4086</v>
+        <v>186.41</v>
       </c>
       <c r="CN116" t="n">
-        <v>196.1324</v>
+        <v>196.13</v>
       </c>
       <c r="CO116" t="n">
-        <v>4.7667</v>
+        <v>4.77</v>
       </c>
       <c r="CP116" t="n">
-        <v>3.5171</v>
+        <v>3.52</v>
       </c>
     </row>
     <row r="117">
@@ -17985,16 +17985,16 @@
       </c>
       <c r="BB118" t="inlineStr"/>
       <c r="BC118" t="n">
-        <v>12.9383</v>
+        <v>12.94</v>
       </c>
       <c r="BD118" t="n">
-        <v>62.0316</v>
+        <v>62.03</v>
       </c>
       <c r="BE118" t="n">
-        <v>80.1212</v>
+        <v>80.12</v>
       </c>
       <c r="BF118" t="n">
-        <v>575.4521</v>
+        <v>575.45</v>
       </c>
       <c r="BG118" t="inlineStr"/>
       <c r="BH118" t="inlineStr"/>
@@ -18029,16 +18029,16 @@
       <c r="CK118" t="inlineStr"/>
       <c r="CL118" t="inlineStr"/>
       <c r="CM118" t="n">
-        <v>219.3832</v>
+        <v>219.38</v>
       </c>
       <c r="CN118" t="n">
-        <v>267.1413</v>
+        <v>267.14</v>
       </c>
       <c r="CO118" t="n">
-        <v>196.3874</v>
+        <v>196.39</v>
       </c>
       <c r="CP118" t="n">
-        <v>201.0302</v>
+        <v>201.03</v>
       </c>
     </row>
     <row r="119">
@@ -18590,10 +18590,10 @@
       <c r="BB122" t="inlineStr"/>
       <c r="BC122" t="inlineStr"/>
       <c r="BD122" t="n">
-        <v>89.27770000000001</v>
+        <v>89.28</v>
       </c>
       <c r="BE122" t="n">
-        <v>95.839</v>
+        <v>95.84</v>
       </c>
       <c r="BF122" t="n">
         <v>85.98</v>
@@ -18631,16 +18631,16 @@
       <c r="CK122" t="inlineStr"/>
       <c r="CL122" t="inlineStr"/>
       <c r="CM122" t="n">
-        <v>197.0112</v>
+        <v>197.01</v>
       </c>
       <c r="CN122" t="n">
-        <v>205.8924</v>
+        <v>205.89</v>
       </c>
       <c r="CO122" t="n">
-        <v>175.9873</v>
+        <v>175.99</v>
       </c>
       <c r="CP122" t="n">
-        <v>190.2007</v>
+        <v>190.2</v>
       </c>
     </row>
     <row r="123">
@@ -19232,13 +19232,13 @@
       <c r="BL126" t="inlineStr"/>
       <c r="BM126" t="inlineStr"/>
       <c r="BN126" t="n">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="BO126" t="n">
-        <v>264.8121</v>
+        <v>264.81</v>
       </c>
       <c r="BP126" t="n">
-        <v>916409.7336999999</v>
+        <v>916409.73</v>
       </c>
       <c r="BQ126" t="inlineStr"/>
       <c r="BR126" t="inlineStr"/>
@@ -19263,16 +19263,16 @@
       <c r="CK126" t="inlineStr"/>
       <c r="CL126" t="inlineStr"/>
       <c r="CM126" t="n">
-        <v>162045.5936</v>
+        <v>162045.59</v>
       </c>
       <c r="CN126" t="n">
-        <v>40.0417</v>
+        <v>40.04</v>
       </c>
       <c r="CO126" t="n">
-        <v>63.641</v>
+        <v>63.64</v>
       </c>
       <c r="CP126" t="n">
-        <v>9301.0129</v>
+        <v>9301.01</v>
       </c>
     </row>
     <row r="127">
@@ -19404,13 +19404,13 @@
       <c r="BJ127" t="inlineStr"/>
       <c r="BK127" t="inlineStr"/>
       <c r="BL127" t="n">
-        <v>136.2488</v>
+        <v>136.25</v>
       </c>
       <c r="BM127" t="n">
-        <v>131.7333</v>
+        <v>131.73</v>
       </c>
       <c r="BN127" t="n">
-        <v>128.158</v>
+        <v>128.16</v>
       </c>
       <c r="BO127" t="inlineStr"/>
       <c r="BP127" t="inlineStr"/>
@@ -19437,16 +19437,16 @@
       <c r="CK127" t="inlineStr"/>
       <c r="CL127" t="inlineStr"/>
       <c r="CM127" t="n">
-        <v>153.6441</v>
+        <v>153.64</v>
       </c>
       <c r="CN127" t="n">
-        <v>123.9354</v>
+        <v>123.94</v>
       </c>
       <c r="CO127" t="n">
-        <v>86.30670000000001</v>
+        <v>86.31</v>
       </c>
       <c r="CP127" t="n">
-        <v>169.894</v>
+        <v>169.89</v>
       </c>
     </row>
     <row r="128">
@@ -21656,16 +21656,16 @@
         <v>2004</v>
       </c>
       <c r="BB142" t="n">
-        <v>2498.3966</v>
+        <v>2498.4</v>
       </c>
       <c r="BC142" t="n">
-        <v>2498.5495</v>
+        <v>2498.55</v>
       </c>
       <c r="BD142" t="n">
-        <v>2699.1466</v>
+        <v>2699.15</v>
       </c>
       <c r="BE142" t="n">
-        <v>2686.495899999999</v>
+        <v>2686.5</v>
       </c>
       <c r="BF142" t="inlineStr"/>
       <c r="BG142" t="inlineStr"/>
@@ -21701,16 +21701,16 @@
       <c r="CK142" t="inlineStr"/>
       <c r="CL142" t="inlineStr"/>
       <c r="CM142" t="n">
-        <v>2685.724099999999</v>
+        <v>2685.72</v>
       </c>
       <c r="CN142" t="n">
-        <v>2685.0131</v>
+        <v>2685.01</v>
       </c>
       <c r="CO142" t="n">
-        <v>2646.4352</v>
+        <v>2646.44</v>
       </c>
       <c r="CP142" t="n">
-        <v>2645.4137</v>
+        <v>2645.41</v>
       </c>
     </row>
     <row r="143">
@@ -21814,16 +21814,16 @@
         <v>2004</v>
       </c>
       <c r="BB143" t="n">
-        <v>14.319</v>
+        <v>14.32</v>
       </c>
       <c r="BC143" t="n">
-        <v>15.6593</v>
+        <v>15.66</v>
       </c>
       <c r="BD143" t="n">
-        <v>41.997</v>
+        <v>42</v>
       </c>
       <c r="BE143" t="n">
-        <v>82.3274</v>
+        <v>82.33</v>
       </c>
       <c r="BF143" t="inlineStr"/>
       <c r="BG143" t="inlineStr"/>
@@ -21859,16 +21859,16 @@
       <c r="CK143" t="inlineStr"/>
       <c r="CL143" t="inlineStr"/>
       <c r="CM143" t="n">
-        <v>29.0442</v>
+        <v>29.04</v>
       </c>
       <c r="CN143" t="n">
-        <v>22.6231</v>
+        <v>22.62</v>
       </c>
       <c r="CO143" t="n">
-        <v>17.7205</v>
+        <v>17.72</v>
       </c>
       <c r="CP143" t="n">
-        <v>15.2777</v>
+        <v>15.28</v>
       </c>
     </row>
     <row r="144">
@@ -21972,16 +21972,16 @@
         <v>2004</v>
       </c>
       <c r="BB144" t="n">
-        <v>108.2251</v>
+        <v>108.23</v>
       </c>
       <c r="BC144" t="n">
-        <v>118.7603</v>
+        <v>118.76</v>
       </c>
       <c r="BD144" t="n">
-        <v>135.1119</v>
+        <v>135.11</v>
       </c>
       <c r="BE144" t="n">
-        <v>96.3013</v>
+        <v>96.3</v>
       </c>
       <c r="BF144" t="inlineStr"/>
       <c r="BG144" t="inlineStr"/>
@@ -22017,16 +22017,16 @@
       <c r="CK144" t="inlineStr"/>
       <c r="CL144" t="inlineStr"/>
       <c r="CM144" t="n">
-        <v>100.1834</v>
+        <v>100.18</v>
       </c>
       <c r="CN144" t="n">
-        <v>78.6079</v>
+        <v>78.61</v>
       </c>
       <c r="CO144" t="n">
-        <v>90.2526</v>
+        <v>90.25</v>
       </c>
       <c r="CP144" t="n">
-        <v>76.9706</v>
+        <v>76.97</v>
       </c>
     </row>
     <row r="145">
@@ -22423,13 +22423,13 @@
         <v>211.04</v>
       </c>
       <c r="BC147" t="n">
-        <v>221.7245</v>
+        <v>221.72</v>
       </c>
       <c r="BD147" t="n">
-        <v>348.9503</v>
+        <v>348.95</v>
       </c>
       <c r="BE147" t="n">
-        <v>276.1723</v>
+        <v>276.17</v>
       </c>
       <c r="BF147" t="inlineStr"/>
       <c r="BG147" t="inlineStr"/>
@@ -22465,16 +22465,16 @@
       <c r="CK147" t="inlineStr"/>
       <c r="CL147" t="inlineStr"/>
       <c r="CM147" t="n">
-        <v>276.1723</v>
+        <v>276.17</v>
       </c>
       <c r="CN147" t="n">
-        <v>336.542</v>
+        <v>336.54</v>
       </c>
       <c r="CO147" t="n">
-        <v>274.6382</v>
+        <v>274.64</v>
       </c>
       <c r="CP147" t="n">
-        <v>169.0576</v>
+        <v>169.06</v>
       </c>
     </row>
     <row r="148">
@@ -22874,16 +22874,16 @@
         <v>2004</v>
       </c>
       <c r="BB150" t="n">
-        <v>16.2762</v>
+        <v>16.28</v>
       </c>
       <c r="BC150" t="n">
-        <v>8.048</v>
+        <v>8.050000000000001</v>
       </c>
       <c r="BD150" t="n">
-        <v>1.5181</v>
+        <v>1.52</v>
       </c>
       <c r="BE150" t="n">
-        <v>2.1693</v>
+        <v>2.17</v>
       </c>
       <c r="BF150" t="inlineStr"/>
       <c r="BG150" t="inlineStr"/>
@@ -22919,16 +22919,16 @@
       <c r="CK150" t="inlineStr"/>
       <c r="CL150" t="inlineStr"/>
       <c r="CM150" t="n">
-        <v>2.1693</v>
+        <v>2.17</v>
       </c>
       <c r="CN150" t="n">
-        <v>21.2192</v>
+        <v>21.22</v>
       </c>
       <c r="CO150" t="n">
-        <v>11.9308</v>
+        <v>11.93</v>
       </c>
       <c r="CP150" t="n">
-        <v>14.209</v>
+        <v>14.21</v>
       </c>
     </row>
     <row r="151">
@@ -24380,10 +24380,10 @@
       <c r="BF160" t="inlineStr"/>
       <c r="BG160" t="inlineStr"/>
       <c r="BH160" t="n">
-        <v>48.8003</v>
+        <v>48.8</v>
       </c>
       <c r="BI160" t="n">
-        <v>186.4086</v>
+        <v>186.41</v>
       </c>
       <c r="BJ160" t="inlineStr"/>
       <c r="BK160" t="inlineStr"/>
@@ -24415,16 +24415,16 @@
       <c r="CK160" t="inlineStr"/>
       <c r="CL160" t="inlineStr"/>
       <c r="CM160" t="n">
-        <v>196.1324</v>
+        <v>196.13</v>
       </c>
       <c r="CN160" t="n">
-        <v>4.7667</v>
+        <v>4.77</v>
       </c>
       <c r="CO160" t="n">
-        <v>3.5171</v>
+        <v>3.52</v>
       </c>
       <c r="CP160" t="n">
-        <v>31.4878</v>
+        <v>31.49</v>
       </c>
     </row>
     <row r="161">
@@ -25243,10 +25243,10 @@
       <c r="BC166" t="inlineStr"/>
       <c r="BD166" t="inlineStr"/>
       <c r="BE166" t="n">
-        <v>2.7697</v>
+        <v>2.77</v>
       </c>
       <c r="BF166" t="n">
-        <v>12.1655</v>
+        <v>12.17</v>
       </c>
       <c r="BG166" t="inlineStr"/>
       <c r="BH166" t="inlineStr"/>
@@ -25281,16 +25281,16 @@
       <c r="CK166" t="inlineStr"/>
       <c r="CL166" t="inlineStr"/>
       <c r="CM166" t="n">
-        <v>4.610300000000001</v>
+        <v>4.61</v>
       </c>
       <c r="CN166" t="n">
-        <v>2.0826</v>
+        <v>2.08</v>
       </c>
       <c r="CO166" t="n">
-        <v>0.0242</v>
+        <v>0.02</v>
       </c>
       <c r="CP166" t="n">
-        <v>0.0002</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167">
@@ -25398,22 +25398,22 @@
         <v>2006</v>
       </c>
       <c r="BB167" t="n">
-        <v>663.8512000000001</v>
+        <v>663.85</v>
       </c>
       <c r="BC167" t="n">
-        <v>341.7916999999999</v>
+        <v>341.79</v>
       </c>
       <c r="BD167" t="n">
-        <v>341.9413999999999</v>
+        <v>341.94</v>
       </c>
       <c r="BE167" t="n">
-        <v>342.0137999999999</v>
+        <v>342.01</v>
       </c>
       <c r="BF167" t="n">
-        <v>1056.2626</v>
+        <v>1056.26</v>
       </c>
       <c r="BG167" t="n">
-        <v>1056.4699</v>
+        <v>1056.47</v>
       </c>
       <c r="BH167" t="inlineStr"/>
       <c r="BI167" t="inlineStr"/>
@@ -25447,16 +25447,16 @@
       <c r="CK167" t="inlineStr"/>
       <c r="CL167" t="inlineStr"/>
       <c r="CM167" t="n">
-        <v>1251.0251</v>
+        <v>1251.03</v>
       </c>
       <c r="CN167" t="n">
-        <v>109.7551</v>
+        <v>109.76</v>
       </c>
       <c r="CO167" t="n">
-        <v>1294.8031</v>
+        <v>1294.8</v>
       </c>
       <c r="CP167" t="n">
-        <v>124.9605</v>
+        <v>124.96</v>
       </c>
     </row>
     <row r="168">
@@ -25570,22 +25570,22 @@
       <c r="BB168" t="inlineStr"/>
       <c r="BC168" t="inlineStr"/>
       <c r="BD168" t="n">
-        <v>111.8811</v>
+        <v>111.88</v>
       </c>
       <c r="BE168" t="n">
-        <v>122.6927</v>
+        <v>122.69</v>
       </c>
       <c r="BF168" t="n">
-        <v>131.0815</v>
+        <v>131.08</v>
       </c>
       <c r="BG168" t="n">
-        <v>119.3817</v>
+        <v>119.38</v>
       </c>
       <c r="BH168" t="n">
-        <v>73.2059</v>
+        <v>73.20999999999999</v>
       </c>
       <c r="BI168" t="n">
-        <v>64.1358</v>
+        <v>64.14</v>
       </c>
       <c r="BJ168" t="inlineStr"/>
       <c r="BK168" t="inlineStr"/>
@@ -25617,16 +25617,16 @@
       <c r="CK168" t="inlineStr"/>
       <c r="CL168" t="inlineStr"/>
       <c r="CM168" t="n">
-        <v>220.7554</v>
+        <v>220.76</v>
       </c>
       <c r="CN168" t="n">
-        <v>214.9861</v>
+        <v>214.99</v>
       </c>
       <c r="CO168" t="n">
-        <v>194.9338</v>
+        <v>194.93</v>
       </c>
       <c r="CP168" t="n">
-        <v>171.7455</v>
+        <v>171.74</v>
       </c>
     </row>
     <row r="169">
@@ -27039,19 +27039,19 @@
         <v>0</v>
       </c>
       <c r="BO177" t="n">
-        <v>1139.9055</v>
+        <v>1139.91</v>
       </c>
       <c r="BP177" t="n">
-        <v>1181.2303</v>
+        <v>1181.23</v>
       </c>
       <c r="BQ177" t="n">
-        <v>1169.4469</v>
+        <v>1169.45</v>
       </c>
       <c r="BR177" t="n">
-        <v>122.1799</v>
+        <v>122.18</v>
       </c>
       <c r="BS177" t="n">
-        <v>219.0001</v>
+        <v>219</v>
       </c>
       <c r="BT177" t="inlineStr"/>
       <c r="BU177" t="inlineStr"/>
@@ -27073,16 +27073,16 @@
       <c r="CK177" t="inlineStr"/>
       <c r="CL177" t="inlineStr"/>
       <c r="CM177" t="n">
-        <v>6568.448300000001</v>
+        <v>6568.45</v>
       </c>
       <c r="CN177" t="n">
-        <v>506.8975</v>
+        <v>506.9</v>
       </c>
       <c r="CO177" t="n">
-        <v>464.6826</v>
+        <v>464.68</v>
       </c>
       <c r="CP177" t="n">
-        <v>640.9975000000001</v>
+        <v>641</v>
       </c>
     </row>
     <row r="178">
@@ -29368,16 +29368,16 @@
         <v>2007</v>
       </c>
       <c r="BB192" t="n">
-        <v>153.2823</v>
+        <v>153.28</v>
       </c>
       <c r="BC192" t="n">
-        <v>156.484</v>
+        <v>156.48</v>
       </c>
       <c r="BD192" t="n">
-        <v>91.44119999999999</v>
+        <v>91.44</v>
       </c>
       <c r="BE192" t="n">
-        <v>95.16969999999999</v>
+        <v>95.17</v>
       </c>
       <c r="BF192" t="inlineStr"/>
       <c r="BG192" t="inlineStr"/>
@@ -29413,16 +29413,16 @@
       <c r="CK192" t="inlineStr"/>
       <c r="CL192" t="inlineStr"/>
       <c r="CM192" t="n">
-        <v>95.16969999999999</v>
+        <v>95.17</v>
       </c>
       <c r="CN192" t="n">
-        <v>112.9355</v>
+        <v>112.94</v>
       </c>
       <c r="CO192" t="n">
-        <v>123.5153</v>
+        <v>123.52</v>
       </c>
       <c r="CP192" t="n">
-        <v>108.7806</v>
+        <v>108.78</v>
       </c>
     </row>
     <row r="193">
@@ -29526,16 +29526,16 @@
         <v>2007</v>
       </c>
       <c r="BB193" t="n">
-        <v>17.9776</v>
+        <v>17.98</v>
       </c>
       <c r="BC193" t="n">
-        <v>17.9776</v>
+        <v>17.98</v>
       </c>
       <c r="BD193" t="n">
-        <v>17.9776</v>
+        <v>17.98</v>
       </c>
       <c r="BE193" t="n">
-        <v>17.9776</v>
+        <v>17.98</v>
       </c>
       <c r="BF193" t="inlineStr"/>
       <c r="BG193" t="inlineStr"/>
@@ -29571,16 +29571,16 @@
       <c r="CK193" t="inlineStr"/>
       <c r="CL193" t="inlineStr"/>
       <c r="CM193" t="n">
-        <v>17.9776</v>
+        <v>17.98</v>
       </c>
       <c r="CN193" t="n">
-        <v>9248.668900000001</v>
+        <v>9248.67</v>
       </c>
       <c r="CO193" t="n">
-        <v>9267.912899999999</v>
+        <v>9267.91</v>
       </c>
       <c r="CP193" t="n">
-        <v>9267.914499999999</v>
+        <v>9267.91</v>
       </c>
     </row>
     <row r="194">
@@ -30290,16 +30290,16 @@
       <c r="BD198" t="inlineStr"/>
       <c r="BE198" t="inlineStr"/>
       <c r="BF198" t="n">
-        <v>62.5274</v>
+        <v>62.53</v>
       </c>
       <c r="BG198" t="n">
-        <v>57.2501</v>
+        <v>57.25</v>
       </c>
       <c r="BH198" t="n">
-        <v>126.4626</v>
+        <v>126.46</v>
       </c>
       <c r="BI198" t="n">
-        <v>280.4459</v>
+        <v>280.45</v>
       </c>
       <c r="BJ198" t="inlineStr"/>
       <c r="BK198" t="inlineStr"/>
@@ -30331,16 +30331,16 @@
       <c r="CK198" t="inlineStr"/>
       <c r="CL198" t="inlineStr"/>
       <c r="CM198" t="n">
-        <v>165.2374</v>
+        <v>165.24</v>
       </c>
       <c r="CN198" t="n">
-        <v>150.7401</v>
+        <v>150.74</v>
       </c>
       <c r="CO198" t="n">
-        <v>162.868</v>
+        <v>162.87</v>
       </c>
       <c r="CP198" t="n">
-        <v>152.6307</v>
+        <v>152.63</v>
       </c>
     </row>
     <row r="199">
@@ -30465,16 +30465,16 @@
       <c r="BG199" t="inlineStr"/>
       <c r="BH199" t="inlineStr"/>
       <c r="BI199" t="n">
-        <v>663.8512000000001</v>
+        <v>663.85</v>
       </c>
       <c r="BJ199" t="n">
-        <v>341.7916999999999</v>
+        <v>341.79</v>
       </c>
       <c r="BK199" t="n">
-        <v>341.9413999999999</v>
+        <v>341.94</v>
       </c>
       <c r="BL199" t="n">
-        <v>342.0137999999999</v>
+        <v>342.01</v>
       </c>
       <c r="BM199" t="inlineStr"/>
       <c r="BN199" t="inlineStr"/>
@@ -30503,16 +30503,16 @@
       <c r="CK199" t="inlineStr"/>
       <c r="CL199" t="inlineStr"/>
       <c r="CM199" t="n">
-        <v>1056.2626</v>
+        <v>1056.26</v>
       </c>
       <c r="CN199" t="n">
-        <v>1056.4699</v>
+        <v>1056.47</v>
       </c>
       <c r="CO199" t="n">
-        <v>1251.0251</v>
+        <v>1251.03</v>
       </c>
       <c r="CP199" t="n">
-        <v>109.7551</v>
+        <v>109.76</v>
       </c>
     </row>
     <row r="200">
@@ -30906,16 +30906,16 @@
         <v>2005</v>
       </c>
       <c r="BB202" t="n">
-        <v>183.4394</v>
+        <v>183.44</v>
       </c>
       <c r="BC202" t="n">
-        <v>173.5015</v>
+        <v>173.5</v>
       </c>
       <c r="BD202" t="n">
-        <v>185.6163</v>
+        <v>185.62</v>
       </c>
       <c r="BE202" t="n">
-        <v>177.9018</v>
+        <v>177.9</v>
       </c>
       <c r="BF202" t="inlineStr"/>
       <c r="BG202" t="inlineStr"/>
@@ -30951,16 +30951,16 @@
       <c r="CK202" t="inlineStr"/>
       <c r="CL202" t="inlineStr"/>
       <c r="CM202" t="n">
-        <v>145.5293</v>
+        <v>145.53</v>
       </c>
       <c r="CN202" t="n">
-        <v>99.5727</v>
+        <v>99.56999999999999</v>
       </c>
       <c r="CO202" t="n">
-        <v>92.84379999999999</v>
+        <v>92.84</v>
       </c>
       <c r="CP202" t="n">
-        <v>219.6253</v>
+        <v>219.63</v>
       </c>
     </row>
     <row r="203">
@@ -31357,10 +31357,10 @@
       <c r="BC205" t="inlineStr"/>
       <c r="BD205" t="inlineStr"/>
       <c r="BE205" t="n">
-        <v>320.4450000000001</v>
+        <v>320.45</v>
       </c>
       <c r="BF205" t="n">
-        <v>285.7957</v>
+        <v>285.8</v>
       </c>
       <c r="BG205" t="inlineStr"/>
       <c r="BH205" t="inlineStr"/>
@@ -31398,13 +31398,13 @@
         <v>114.08</v>
       </c>
       <c r="CN205" t="n">
-        <v>163.494</v>
+        <v>163.49</v>
       </c>
       <c r="CO205" t="n">
-        <v>143.3225</v>
+        <v>143.32</v>
       </c>
       <c r="CP205" t="n">
-        <v>2216.1232</v>
+        <v>2216.12</v>
       </c>
     </row>
     <row r="206">
@@ -31984,22 +31984,22 @@
         <v>2006</v>
       </c>
       <c r="BB209" t="n">
-        <v>28.4083</v>
+        <v>28.41</v>
       </c>
       <c r="BC209" t="n">
-        <v>32.5894</v>
+        <v>32.59</v>
       </c>
       <c r="BD209" t="n">
-        <v>46.6483</v>
+        <v>46.65</v>
       </c>
       <c r="BE209" t="n">
-        <v>46.5694</v>
+        <v>46.57</v>
       </c>
       <c r="BF209" t="n">
-        <v>42.6264</v>
+        <v>42.63</v>
       </c>
       <c r="BG209" t="n">
-        <v>43.3766</v>
+        <v>43.38</v>
       </c>
       <c r="BH209" t="inlineStr"/>
       <c r="BI209" t="inlineStr"/>
@@ -32033,16 +32033,16 @@
       <c r="CK209" t="inlineStr"/>
       <c r="CL209" t="inlineStr"/>
       <c r="CM209" t="n">
-        <v>48.1665</v>
+        <v>48.17</v>
       </c>
       <c r="CN209" t="n">
-        <v>50.5589</v>
+        <v>50.56</v>
       </c>
       <c r="CO209" t="n">
-        <v>48.3146</v>
+        <v>48.31</v>
       </c>
       <c r="CP209" t="n">
-        <v>48.8719</v>
+        <v>48.87</v>
       </c>
     </row>
     <row r="210">
@@ -32158,25 +32158,25 @@
       <c r="BB210" t="inlineStr"/>
       <c r="BC210" t="inlineStr"/>
       <c r="BD210" t="n">
-        <v>663.8512000000001</v>
+        <v>663.85</v>
       </c>
       <c r="BE210" t="n">
-        <v>341.7916999999999</v>
+        <v>341.79</v>
       </c>
       <c r="BF210" t="n">
-        <v>341.9413999999999</v>
+        <v>341.94</v>
       </c>
       <c r="BG210" t="n">
-        <v>342.0137999999999</v>
+        <v>342.01</v>
       </c>
       <c r="BH210" t="n">
-        <v>1056.2626</v>
+        <v>1056.26</v>
       </c>
       <c r="BI210" t="n">
-        <v>1056.4699</v>
+        <v>1056.47</v>
       </c>
       <c r="BJ210" t="n">
-        <v>1251.0251</v>
+        <v>1251.03</v>
       </c>
       <c r="BK210" t="inlineStr"/>
       <c r="BL210" t="inlineStr"/>
@@ -32207,16 +32207,16 @@
       <c r="CK210" t="inlineStr"/>
       <c r="CL210" t="inlineStr"/>
       <c r="CM210" t="n">
-        <v>109.7551</v>
+        <v>109.76</v>
       </c>
       <c r="CN210" t="n">
-        <v>1294.8031</v>
+        <v>1294.8</v>
       </c>
       <c r="CO210" t="n">
-        <v>124.9605</v>
+        <v>124.96</v>
       </c>
       <c r="CP210" t="n">
-        <v>950.6646000000001</v>
+        <v>950.66</v>
       </c>
     </row>
     <row r="211">
@@ -32657,25 +32657,25 @@
       <c r="BG213" t="inlineStr"/>
       <c r="BH213" t="inlineStr"/>
       <c r="BI213" t="n">
-        <v>444.2461000000001</v>
+        <v>444.25</v>
       </c>
       <c r="BJ213" t="n">
-        <v>459.8627</v>
+        <v>459.86</v>
       </c>
       <c r="BK213" t="n">
-        <v>41.1298</v>
+        <v>41.13</v>
       </c>
       <c r="BL213" t="n">
-        <v>33.3318</v>
+        <v>33.33</v>
       </c>
       <c r="BM213" t="n">
-        <v>29.0056</v>
+        <v>29.01</v>
       </c>
       <c r="BN213" t="n">
-        <v>126.983</v>
+        <v>126.98</v>
       </c>
       <c r="BO213" t="n">
-        <v>44.9481</v>
+        <v>44.95</v>
       </c>
       <c r="BP213" t="inlineStr"/>
       <c r="BQ213" t="inlineStr"/>
@@ -32701,16 +32701,16 @@
       <c r="CK213" t="inlineStr"/>
       <c r="CL213" t="inlineStr"/>
       <c r="CM213" t="n">
-        <v>54.1575</v>
+        <v>54.16</v>
       </c>
       <c r="CN213" t="n">
-        <v>61.721</v>
+        <v>61.72</v>
       </c>
       <c r="CO213" t="n">
-        <v>22.1811</v>
+        <v>22.18</v>
       </c>
       <c r="CP213" t="n">
-        <v>51.4251</v>
+        <v>51.43</v>
       </c>
     </row>
     <row r="214">
@@ -32863,16 +32863,16 @@
       <c r="CK214" t="inlineStr"/>
       <c r="CL214" t="inlineStr"/>
       <c r="CM214" t="n">
-        <v>224.4613</v>
+        <v>224.46</v>
       </c>
       <c r="CN214" t="n">
-        <v>360.3223</v>
+        <v>360.32</v>
       </c>
       <c r="CO214" t="n">
-        <v>340.0982</v>
+        <v>340.1</v>
       </c>
       <c r="CP214" t="n">
-        <v>437.0939</v>
+        <v>437.09</v>
       </c>
     </row>
     <row r="215">
@@ -33124,13 +33124,13 @@
         <v>0</v>
       </c>
       <c r="BD216" t="n">
-        <v>0.2033</v>
+        <v>0.2</v>
       </c>
       <c r="BE216" t="n">
-        <v>1449.0285</v>
+        <v>1449.03</v>
       </c>
       <c r="BF216" t="n">
-        <v>1645.8248</v>
+        <v>1645.82</v>
       </c>
       <c r="BG216" t="inlineStr"/>
       <c r="BH216" t="inlineStr"/>
@@ -33165,16 +33165,16 @@
       <c r="CK216" t="inlineStr"/>
       <c r="CL216" t="inlineStr"/>
       <c r="CM216" t="n">
-        <v>1657.1109</v>
+        <v>1657.11</v>
       </c>
       <c r="CN216" t="n">
-        <v>2112.0477</v>
+        <v>2112.05</v>
       </c>
       <c r="CO216" t="n">
-        <v>2114.1062</v>
+        <v>2114.11</v>
       </c>
       <c r="CP216" t="n">
-        <v>2803.5143</v>
+        <v>2803.51</v>
       </c>
     </row>
     <row r="217">
@@ -33430,19 +33430,19 @@
       <c r="BB218" t="inlineStr"/>
       <c r="BC218" t="inlineStr"/>
       <c r="BD218" t="n">
-        <v>198.6875</v>
+        <v>198.69</v>
       </c>
       <c r="BE218" t="n">
-        <v>192.9172</v>
+        <v>192.92</v>
       </c>
       <c r="BF218" t="n">
-        <v>162.4484</v>
+        <v>162.45</v>
       </c>
       <c r="BG218" t="n">
-        <v>156.5363</v>
+        <v>156.54</v>
       </c>
       <c r="BH218" t="n">
-        <v>153.2823</v>
+        <v>153.28</v>
       </c>
       <c r="BI218" t="inlineStr"/>
       <c r="BJ218" t="inlineStr"/>
@@ -33475,16 +33475,16 @@
       <c r="CK218" t="inlineStr"/>
       <c r="CL218" t="inlineStr"/>
       <c r="CM218" t="n">
-        <v>156.484</v>
+        <v>156.48</v>
       </c>
       <c r="CN218" t="n">
-        <v>91.44119999999999</v>
+        <v>91.44</v>
       </c>
       <c r="CO218" t="n">
-        <v>95.16969999999999</v>
+        <v>95.17</v>
       </c>
       <c r="CP218" t="n">
-        <v>112.9355</v>
+        <v>112.94</v>
       </c>
     </row>
     <row r="219">
@@ -33605,10 +33605,10 @@
         <v>0</v>
       </c>
       <c r="BG219" t="n">
-        <v>18.4041</v>
+        <v>18.4</v>
       </c>
       <c r="BH219" t="n">
-        <v>17.9776</v>
+        <v>17.98</v>
       </c>
       <c r="BI219" t="inlineStr"/>
       <c r="BJ219" t="inlineStr"/>
@@ -33641,16 +33641,16 @@
       <c r="CK219" t="inlineStr"/>
       <c r="CL219" t="inlineStr"/>
       <c r="CM219" t="n">
-        <v>17.9776</v>
+        <v>17.98</v>
       </c>
       <c r="CN219" t="n">
-        <v>17.9776</v>
+        <v>17.98</v>
       </c>
       <c r="CO219" t="n">
-        <v>17.9776</v>
+        <v>17.98</v>
       </c>
       <c r="CP219" t="n">
-        <v>9248.668900000001</v>
+        <v>9248.67</v>
       </c>
     </row>
     <row r="220">
@@ -33941,16 +33941,16 @@
       <c r="CK221" t="inlineStr"/>
       <c r="CL221" t="inlineStr"/>
       <c r="CM221" t="n">
-        <v>3800.3278</v>
+        <v>3800.33</v>
       </c>
       <c r="CN221" t="n">
-        <v>155.6239</v>
+        <v>155.62</v>
       </c>
       <c r="CO221" t="n">
-        <v>138.0622</v>
+        <v>138.06</v>
       </c>
       <c r="CP221" t="n">
-        <v>149.6885</v>
+        <v>149.69</v>
       </c>
     </row>
     <row r="222">
@@ -34059,19 +34059,19 @@
       </c>
       <c r="BB222" t="inlineStr"/>
       <c r="BC222" t="n">
-        <v>11.8057</v>
+        <v>11.81</v>
       </c>
       <c r="BD222" t="n">
-        <v>12.5071</v>
+        <v>12.51</v>
       </c>
       <c r="BE222" t="n">
-        <v>16.727</v>
+        <v>16.73</v>
       </c>
       <c r="BF222" t="n">
-        <v>57.9489</v>
+        <v>57.95</v>
       </c>
       <c r="BG222" t="n">
-        <v>59.05670000000001</v>
+        <v>59.06</v>
       </c>
       <c r="BH222" t="inlineStr"/>
       <c r="BI222" t="inlineStr"/>
@@ -34105,13 +34105,13 @@
       <c r="CK222" t="inlineStr"/>
       <c r="CL222" t="inlineStr"/>
       <c r="CM222" t="n">
-        <v>53.6299</v>
+        <v>53.63</v>
       </c>
       <c r="CN222" t="n">
-        <v>52.32580000000001</v>
+        <v>52.33</v>
       </c>
       <c r="CO222" t="n">
-        <v>51.7539</v>
+        <v>51.75</v>
       </c>
       <c r="CP222" t="n">
         <v>55.37</v>
@@ -34232,10 +34232,10 @@
         <v>0</v>
       </c>
       <c r="BF223" t="n">
-        <v>0.1489</v>
+        <v>0.15</v>
       </c>
       <c r="BG223" t="n">
-        <v>9.628200000000001</v>
+        <v>9.630000000000001</v>
       </c>
       <c r="BH223" t="inlineStr"/>
       <c r="BI223" t="inlineStr"/>
@@ -34269,16 +34269,16 @@
       <c r="CK223" t="inlineStr"/>
       <c r="CL223" t="inlineStr"/>
       <c r="CM223" t="n">
-        <v>29.4781</v>
+        <v>29.48</v>
       </c>
       <c r="CN223" t="n">
-        <v>12.9454</v>
+        <v>12.95</v>
       </c>
       <c r="CO223" t="n">
-        <v>10.8216</v>
+        <v>10.82</v>
       </c>
       <c r="CP223" t="n">
-        <v>21.2648</v>
+        <v>21.26</v>
       </c>
     </row>
     <row r="224">
@@ -34535,13 +34535,13 @@
         <v>0</v>
       </c>
       <c r="BE225" t="n">
-        <v>4420.920099999999</v>
+        <v>4420.92</v>
       </c>
       <c r="BF225" t="n">
-        <v>4420.921799999999</v>
+        <v>4420.92</v>
       </c>
       <c r="BG225" t="n">
-        <v>0.0017</v>
+        <v>0</v>
       </c>
       <c r="BH225" t="inlineStr"/>
       <c r="BI225" t="inlineStr"/>
@@ -34693,19 +34693,19 @@
       </c>
       <c r="BB226" t="inlineStr"/>
       <c r="BC226" t="n">
-        <v>199.3944</v>
+        <v>199.39</v>
       </c>
       <c r="BD226" t="n">
-        <v>208.3569</v>
+        <v>208.36</v>
       </c>
       <c r="BE226" t="n">
-        <v>214.8597</v>
+        <v>214.86</v>
       </c>
       <c r="BF226" t="n">
-        <v>223.9847</v>
+        <v>223.98</v>
       </c>
       <c r="BG226" t="n">
-        <v>221.1238</v>
+        <v>221.12</v>
       </c>
       <c r="BH226" t="inlineStr"/>
       <c r="BI226" t="inlineStr"/>
@@ -34739,16 +34739,16 @@
       <c r="CK226" t="inlineStr"/>
       <c r="CL226" t="inlineStr"/>
       <c r="CM226" t="n">
-        <v>187.2125</v>
+        <v>187.21</v>
       </c>
       <c r="CN226" t="n">
-        <v>140.0581</v>
+        <v>140.06</v>
       </c>
       <c r="CO226" t="n">
-        <v>130.4596</v>
+        <v>130.46</v>
       </c>
       <c r="CP226" t="n">
-        <v>169.962</v>
+        <v>169.96</v>
       </c>
     </row>
     <row r="227">
@@ -34999,19 +34999,19 @@
       </c>
       <c r="BB228" t="inlineStr"/>
       <c r="BC228" t="n">
-        <v>70.9679</v>
+        <v>70.97</v>
       </c>
       <c r="BD228" t="n">
-        <v>67.6203</v>
+        <v>67.62</v>
       </c>
       <c r="BE228" t="n">
-        <v>63.1375</v>
+        <v>63.14</v>
       </c>
       <c r="BF228" t="n">
-        <v>61.2654</v>
+        <v>61.27</v>
       </c>
       <c r="BG228" t="n">
-        <v>36.2026</v>
+        <v>36.2</v>
       </c>
       <c r="BH228" t="inlineStr"/>
       <c r="BI228" t="inlineStr"/>
@@ -35045,16 +35045,16 @@
       <c r="CK228" t="inlineStr"/>
       <c r="CL228" t="inlineStr"/>
       <c r="CM228" t="n">
-        <v>51.5634</v>
+        <v>51.56</v>
       </c>
       <c r="CN228" t="n">
-        <v>38.9874</v>
+        <v>38.99</v>
       </c>
       <c r="CO228" t="n">
-        <v>36.9157</v>
+        <v>36.92</v>
       </c>
       <c r="CP228" t="n">
-        <v>42.7282</v>
+        <v>42.73</v>
       </c>
     </row>
     <row r="229">
@@ -35628,13 +35628,13 @@
       <c r="BB232" t="inlineStr"/>
       <c r="BC232" t="inlineStr"/>
       <c r="BD232" t="n">
-        <v>297.0404</v>
+        <v>297.04</v>
       </c>
       <c r="BE232" t="n">
-        <v>183.5927</v>
+        <v>183.59</v>
       </c>
       <c r="BF232" t="n">
-        <v>263.5501</v>
+        <v>263.55</v>
       </c>
       <c r="BG232" t="inlineStr"/>
       <c r="BH232" t="inlineStr"/>
@@ -35669,16 +35669,16 @@
       <c r="CK232" t="inlineStr"/>
       <c r="CL232" t="inlineStr"/>
       <c r="CM232" t="n">
-        <v>324.1991</v>
+        <v>324.2</v>
       </c>
       <c r="CN232" t="n">
-        <v>280.3223</v>
+        <v>280.32</v>
       </c>
       <c r="CO232" t="n">
-        <v>327.7716</v>
+        <v>327.77</v>
       </c>
       <c r="CP232" t="n">
-        <v>363.1373</v>
+        <v>363.14</v>
       </c>
     </row>
     <row r="233">
@@ -35785,16 +35785,16 @@
       </c>
       <c r="BB233" t="inlineStr"/>
       <c r="BC233" t="n">
-        <v>313.2422</v>
+        <v>313.24</v>
       </c>
       <c r="BD233" t="n">
-        <v>283.6726</v>
+        <v>283.67</v>
       </c>
       <c r="BE233" t="n">
-        <v>170.8882</v>
+        <v>170.89</v>
       </c>
       <c r="BF233" t="n">
-        <v>276.8023</v>
+        <v>276.8</v>
       </c>
       <c r="BG233" t="inlineStr"/>
       <c r="BH233" t="inlineStr"/>
@@ -35829,16 +35829,16 @@
       <c r="CK233" t="inlineStr"/>
       <c r="CL233" t="inlineStr"/>
       <c r="CM233" t="n">
-        <v>410.983</v>
+        <v>410.98</v>
       </c>
       <c r="CN233" t="n">
-        <v>423.2789</v>
+        <v>423.28</v>
       </c>
       <c r="CO233" t="n">
-        <v>461.5015</v>
+        <v>461.5</v>
       </c>
       <c r="CP233" t="n">
-        <v>463.5811</v>
+        <v>463.58</v>
       </c>
     </row>
     <row r="234">
@@ -35954,7 +35954,7 @@
         <v>0</v>
       </c>
       <c r="BF234" t="n">
-        <v>5061.244</v>
+        <v>5061.24</v>
       </c>
       <c r="BG234" t="inlineStr"/>
       <c r="BH234" t="inlineStr"/>
@@ -35989,16 +35989,16 @@
       <c r="CK234" t="inlineStr"/>
       <c r="CL234" t="inlineStr"/>
       <c r="CM234" t="n">
-        <v>4124.972900000001</v>
+        <v>4124.97</v>
       </c>
       <c r="CN234" t="n">
-        <v>1294.9582</v>
+        <v>1294.96</v>
       </c>
       <c r="CO234" t="n">
-        <v>1219.0075</v>
+        <v>1219.01</v>
       </c>
       <c r="CP234" t="n">
-        <v>427.241</v>
+        <v>427.24</v>
       </c>
     </row>
     <row r="235">
@@ -36105,16 +36105,16 @@
       </c>
       <c r="BB235" t="inlineStr"/>
       <c r="BC235" t="n">
-        <v>214.0629</v>
+        <v>214.06</v>
       </c>
       <c r="BD235" t="n">
-        <v>151.5227</v>
+        <v>151.52</v>
       </c>
       <c r="BE235" t="n">
-        <v>5016.6278</v>
+        <v>5016.63</v>
       </c>
       <c r="BF235" t="n">
-        <v>108.5281</v>
+        <v>108.53</v>
       </c>
       <c r="BG235" t="inlineStr"/>
       <c r="BH235" t="inlineStr"/>
@@ -36149,16 +36149,16 @@
       <c r="CK235" t="inlineStr"/>
       <c r="CL235" t="inlineStr"/>
       <c r="CM235" t="n">
-        <v>148.9636</v>
+        <v>148.96</v>
       </c>
       <c r="CN235" t="n">
-        <v>83.06310000000001</v>
+        <v>83.06</v>
       </c>
       <c r="CO235" t="n">
-        <v>81.2209</v>
+        <v>81.22</v>
       </c>
       <c r="CP235" t="n">
-        <v>85.46680000000001</v>
+        <v>85.47</v>
       </c>
     </row>
     <row r="236">
@@ -36316,7 +36316,7 @@
         <v>0</v>
       </c>
       <c r="CP236" t="n">
-        <v>1252.3986</v>
+        <v>1252.4</v>
       </c>
     </row>
     <row r="237">
@@ -36423,16 +36423,16 @@
       </c>
       <c r="BB237" t="inlineStr"/>
       <c r="BC237" t="n">
-        <v>97.32679999999999</v>
+        <v>97.33</v>
       </c>
       <c r="BD237" t="n">
-        <v>119.3765</v>
+        <v>119.38</v>
       </c>
       <c r="BE237" t="n">
-        <v>58.0534</v>
+        <v>58.05</v>
       </c>
       <c r="BF237" t="n">
-        <v>79.30540000000001</v>
+        <v>79.31</v>
       </c>
       <c r="BG237" t="inlineStr"/>
       <c r="BH237" t="inlineStr"/>
@@ -36467,16 +36467,16 @@
       <c r="CK237" t="inlineStr"/>
       <c r="CL237" t="inlineStr"/>
       <c r="CM237" t="n">
-        <v>98.02379999999999</v>
+        <v>98.02</v>
       </c>
       <c r="CN237" t="n">
-        <v>87.28920000000001</v>
+        <v>87.29000000000001</v>
       </c>
       <c r="CO237" t="n">
-        <v>163.8368</v>
+        <v>163.84</v>
       </c>
       <c r="CP237" t="n">
-        <v>134.2245</v>
+        <v>134.22</v>
       </c>
     </row>
     <row r="238">
@@ -36583,16 +36583,16 @@
       </c>
       <c r="BB238" t="inlineStr"/>
       <c r="BC238" t="n">
-        <v>38.0819</v>
+        <v>38.08</v>
       </c>
       <c r="BD238" t="n">
-        <v>46.1934</v>
+        <v>46.19</v>
       </c>
       <c r="BE238" t="n">
-        <v>66.5686</v>
+        <v>66.56999999999999</v>
       </c>
       <c r="BF238" t="n">
-        <v>84.6379</v>
+        <v>84.64</v>
       </c>
       <c r="BG238" t="inlineStr"/>
       <c r="BH238" t="inlineStr"/>
@@ -36627,16 +36627,16 @@
       <c r="CK238" t="inlineStr"/>
       <c r="CL238" t="inlineStr"/>
       <c r="CM238" t="n">
-        <v>78.879</v>
+        <v>78.88</v>
       </c>
       <c r="CN238" t="n">
-        <v>83.8933</v>
+        <v>83.89</v>
       </c>
       <c r="CO238" t="n">
-        <v>101.2604</v>
+        <v>101.26</v>
       </c>
       <c r="CP238" t="n">
-        <v>108.0493</v>
+        <v>108.05</v>
       </c>
     </row>
     <row r="239">
@@ -36743,16 +36743,16 @@
       </c>
       <c r="BB239" t="inlineStr"/>
       <c r="BC239" t="n">
-        <v>70.9679</v>
+        <v>70.97</v>
       </c>
       <c r="BD239" t="n">
-        <v>67.6203</v>
+        <v>67.62</v>
       </c>
       <c r="BE239" t="n">
-        <v>63.1375</v>
+        <v>63.14</v>
       </c>
       <c r="BF239" t="n">
-        <v>61.2654</v>
+        <v>61.27</v>
       </c>
       <c r="BG239" t="inlineStr"/>
       <c r="BH239" t="inlineStr"/>
@@ -36787,16 +36787,16 @@
       <c r="CK239" t="inlineStr"/>
       <c r="CL239" t="inlineStr"/>
       <c r="CM239" t="n">
-        <v>36.2026</v>
+        <v>36.2</v>
       </c>
       <c r="CN239" t="n">
-        <v>51.5634</v>
+        <v>51.56</v>
       </c>
       <c r="CO239" t="n">
-        <v>38.9874</v>
+        <v>38.99</v>
       </c>
       <c r="CP239" t="n">
-        <v>36.9157</v>
+        <v>36.92</v>
       </c>
     </row>
     <row r="240">
@@ -36903,16 +36903,16 @@
       </c>
       <c r="BB240" t="inlineStr"/>
       <c r="BC240" t="n">
-        <v>88.0283</v>
+        <v>88.03</v>
       </c>
       <c r="BD240" t="n">
-        <v>89.6019</v>
+        <v>89.59999999999999</v>
       </c>
       <c r="BE240" t="n">
-        <v>67.4539</v>
+        <v>67.45</v>
       </c>
       <c r="BF240" t="n">
-        <v>71.3001</v>
+        <v>71.3</v>
       </c>
       <c r="BG240" t="inlineStr"/>
       <c r="BH240" t="inlineStr"/>
@@ -36947,16 +36947,16 @@
       <c r="CK240" t="inlineStr"/>
       <c r="CL240" t="inlineStr"/>
       <c r="CM240" t="n">
-        <v>67.76139999999999</v>
+        <v>67.76000000000001</v>
       </c>
       <c r="CN240" t="n">
-        <v>71.61880000000001</v>
+        <v>71.62</v>
       </c>
       <c r="CO240" t="n">
-        <v>60.8053</v>
+        <v>60.81</v>
       </c>
       <c r="CP240" t="n">
-        <v>60.9934</v>
+        <v>60.99</v>
       </c>
     </row>
     <row r="241">
@@ -37066,10 +37066,10 @@
         <v>0</v>
       </c>
       <c r="BD241" t="n">
-        <v>0.1361</v>
+        <v>0.14</v>
       </c>
       <c r="BE241" t="n">
-        <v>2772.3615</v>
+        <v>2772.36</v>
       </c>
       <c r="BF241" t="inlineStr"/>
       <c r="BG241" t="inlineStr"/>
@@ -37105,16 +37105,16 @@
       <c r="CK241" t="inlineStr"/>
       <c r="CL241" t="inlineStr"/>
       <c r="CM241" t="n">
-        <v>2772.3615</v>
+        <v>2772.36</v>
       </c>
       <c r="CN241" t="n">
-        <v>2300.2056</v>
+        <v>2300.21</v>
       </c>
       <c r="CO241" t="n">
-        <v>2093.8748</v>
+        <v>2093.87</v>
       </c>
       <c r="CP241" t="n">
-        <v>2047.3218</v>
+        <v>2047.32</v>
       </c>
     </row>
     <row r="242">
@@ -37556,16 +37556,16 @@
       <c r="BB244" t="inlineStr"/>
       <c r="BC244" t="inlineStr"/>
       <c r="BD244" t="n">
-        <v>2569.355700000001</v>
+        <v>2569.36</v>
       </c>
       <c r="BE244" t="n">
         <v>2339.92</v>
       </c>
       <c r="BF244" t="n">
-        <v>1671.6668</v>
+        <v>1671.67</v>
       </c>
       <c r="BG244" t="n">
-        <v>1677.9539</v>
+        <v>1677.95</v>
       </c>
       <c r="BH244" t="inlineStr"/>
       <c r="BI244" t="inlineStr"/>
@@ -37599,16 +37599,16 @@
       <c r="CK244" t="inlineStr"/>
       <c r="CL244" t="inlineStr"/>
       <c r="CM244" t="n">
-        <v>1615.5437</v>
+        <v>1615.54</v>
       </c>
       <c r="CN244" t="n">
-        <v>1635.4137</v>
+        <v>1635.41</v>
       </c>
       <c r="CO244" t="n">
-        <v>1642.2275</v>
+        <v>1642.23</v>
       </c>
       <c r="CP244" t="n">
-        <v>1615.7754</v>
+        <v>1615.78</v>
       </c>
     </row>
     <row r="245">
@@ -38012,28 +38012,28 @@
         <v>2008</v>
       </c>
       <c r="BB247" t="n">
-        <v>314.3065999999999</v>
+        <v>314.31</v>
       </c>
       <c r="BC247" t="n">
-        <v>78.77019999999999</v>
+        <v>78.77</v>
       </c>
       <c r="BD247" t="n">
-        <v>101.7722</v>
+        <v>101.77</v>
       </c>
       <c r="BE247" t="n">
-        <v>115.7356</v>
+        <v>115.74</v>
       </c>
       <c r="BF247" t="n">
-        <v>156.8433</v>
+        <v>156.84</v>
       </c>
       <c r="BG247" t="n">
-        <v>261.1526</v>
+        <v>261.15</v>
       </c>
       <c r="BH247" t="n">
-        <v>341.1844</v>
+        <v>341.18</v>
       </c>
       <c r="BI247" t="n">
-        <v>184.2922</v>
+        <v>184.29</v>
       </c>
       <c r="BJ247" t="inlineStr"/>
       <c r="BK247" t="inlineStr"/>
@@ -38065,16 +38065,16 @@
       <c r="CK247" t="inlineStr"/>
       <c r="CL247" t="inlineStr"/>
       <c r="CM247" t="n">
-        <v>186.8076</v>
+        <v>186.81</v>
       </c>
       <c r="CN247" t="n">
-        <v>218.1126</v>
+        <v>218.11</v>
       </c>
       <c r="CO247" t="n">
-        <v>330.4024</v>
+        <v>330.4</v>
       </c>
       <c r="CP247" t="n">
-        <v>324.8236</v>
+        <v>324.82</v>
       </c>
     </row>
     <row r="248">
@@ -38186,28 +38186,28 @@
         <v>2008</v>
       </c>
       <c r="BB248" t="n">
-        <v>611.6212</v>
+        <v>611.62</v>
       </c>
       <c r="BC248" t="n">
-        <v>2669.6755</v>
+        <v>2669.68</v>
       </c>
       <c r="BD248" t="n">
-        <v>2675.8751</v>
+        <v>2675.88</v>
       </c>
       <c r="BE248" t="n">
-        <v>2753.2038</v>
+        <v>2753.2</v>
       </c>
       <c r="BF248" t="n">
-        <v>2771.456</v>
+        <v>2771.46</v>
       </c>
       <c r="BG248" t="n">
         <v>2758.94</v>
       </c>
       <c r="BH248" t="n">
-        <v>2784.3183</v>
+        <v>2784.32</v>
       </c>
       <c r="BI248" t="n">
-        <v>2741.6486</v>
+        <v>2741.65</v>
       </c>
       <c r="BJ248" t="inlineStr"/>
       <c r="BK248" t="inlineStr"/>
@@ -38239,16 +38239,16 @@
       <c r="CK248" t="inlineStr"/>
       <c r="CL248" t="inlineStr"/>
       <c r="CM248" t="n">
-        <v>2796.002</v>
+        <v>2796</v>
       </c>
       <c r="CN248" t="n">
-        <v>2060.6542</v>
+        <v>2060.65</v>
       </c>
       <c r="CO248" t="n">
-        <v>2066.155</v>
+        <v>2066.15</v>
       </c>
       <c r="CP248" t="n">
-        <v>2088.0333</v>
+        <v>2088.03</v>
       </c>
     </row>
     <row r="249">
@@ -38360,28 +38360,28 @@
         <v>2008</v>
       </c>
       <c r="BB249" t="n">
-        <v>816.3812</v>
+        <v>816.38</v>
       </c>
       <c r="BC249" t="n">
-        <v>891.5358</v>
+        <v>891.54</v>
       </c>
       <c r="BD249" t="n">
-        <v>854.0382999999999</v>
+        <v>854.04</v>
       </c>
       <c r="BE249" t="n">
-        <v>953.7976</v>
+        <v>953.8</v>
       </c>
       <c r="BF249" t="n">
-        <v>677.9825000000001</v>
+        <v>677.98</v>
       </c>
       <c r="BG249" t="n">
-        <v>464.4476</v>
+        <v>464.45</v>
       </c>
       <c r="BH249" t="n">
-        <v>342.5049</v>
+        <v>342.5</v>
       </c>
       <c r="BI249" t="n">
-        <v>50.05880000000001</v>
+        <v>50.06</v>
       </c>
       <c r="BJ249" t="inlineStr"/>
       <c r="BK249" t="inlineStr"/>
@@ -38413,16 +38413,16 @@
       <c r="CK249" t="inlineStr"/>
       <c r="CL249" t="inlineStr"/>
       <c r="CM249" t="n">
-        <v>79.1339</v>
+        <v>79.13</v>
       </c>
       <c r="CN249" t="n">
-        <v>78.37379999999999</v>
+        <v>78.37</v>
       </c>
       <c r="CO249" t="n">
-        <v>148.4714</v>
+        <v>148.47</v>
       </c>
       <c r="CP249" t="n">
-        <v>365.7021</v>
+        <v>365.7</v>
       </c>
     </row>
     <row r="250">
@@ -38680,28 +38680,28 @@
         <v>2008</v>
       </c>
       <c r="BB251" t="n">
-        <v>2946.4402</v>
+        <v>2946.44</v>
       </c>
       <c r="BC251" t="n">
-        <v>2747.8588</v>
+        <v>2747.86</v>
       </c>
       <c r="BD251" t="n">
-        <v>2705.0035</v>
+        <v>2705</v>
       </c>
       <c r="BE251" t="n">
-        <v>3139.8016</v>
+        <v>3139.8</v>
       </c>
       <c r="BF251" t="n">
-        <v>3233.7821</v>
+        <v>3233.78</v>
       </c>
       <c r="BG251" t="n">
-        <v>3233.4479</v>
+        <v>3233.45</v>
       </c>
       <c r="BH251" t="n">
-        <v>3232.411500000001</v>
+        <v>3232.41</v>
       </c>
       <c r="BI251" t="n">
-        <v>3288.7234</v>
+        <v>3288.72</v>
       </c>
       <c r="BJ251" t="inlineStr"/>
       <c r="BK251" t="inlineStr"/>
@@ -38733,16 +38733,16 @@
       <c r="CK251" t="inlineStr"/>
       <c r="CL251" t="inlineStr"/>
       <c r="CM251" t="n">
-        <v>3245.1082</v>
+        <v>3245.11</v>
       </c>
       <c r="CN251" t="n">
-        <v>3136.0963</v>
+        <v>3136.1</v>
       </c>
       <c r="CO251" t="n">
-        <v>3441.9841</v>
+        <v>3441.98</v>
       </c>
       <c r="CP251" t="n">
-        <v>2984.1227</v>
+        <v>2984.12</v>
       </c>
     </row>
     <row r="252">
@@ -38850,22 +38850,22 @@
         <v>2008</v>
       </c>
       <c r="BB252" t="n">
-        <v>5016.6278</v>
+        <v>5016.63</v>
       </c>
       <c r="BC252" t="n">
-        <v>108.5281</v>
+        <v>108.53</v>
       </c>
       <c r="BD252" t="n">
-        <v>148.9636</v>
+        <v>148.96</v>
       </c>
       <c r="BE252" t="n">
-        <v>83.06310000000001</v>
+        <v>83.06</v>
       </c>
       <c r="BF252" t="n">
-        <v>81.2209</v>
+        <v>81.22</v>
       </c>
       <c r="BG252" t="n">
-        <v>85.46680000000001</v>
+        <v>85.47</v>
       </c>
       <c r="BH252" t="inlineStr"/>
       <c r="BI252" t="inlineStr"/>
@@ -38899,16 +38899,16 @@
       <c r="CK252" t="inlineStr"/>
       <c r="CL252" t="inlineStr"/>
       <c r="CM252" t="n">
-        <v>75.91659999999999</v>
+        <v>75.92</v>
       </c>
       <c r="CN252" t="n">
-        <v>102.9275</v>
+        <v>102.93</v>
       </c>
       <c r="CO252" t="n">
-        <v>117.4392</v>
+        <v>117.44</v>
       </c>
       <c r="CP252" t="n">
-        <v>44.15489999999999</v>
+        <v>44.15</v>
       </c>
     </row>
     <row r="253">
@@ -39031,7 +39031,7 @@
         <v>0</v>
       </c>
       <c r="BG253" t="n">
-        <v>3972.9714</v>
+        <v>3972.97</v>
       </c>
       <c r="BH253" t="inlineStr"/>
       <c r="BI253" t="inlineStr"/>
@@ -39065,16 +39065,16 @@
       <c r="CK253" t="inlineStr"/>
       <c r="CL253" t="inlineStr"/>
       <c r="CM253" t="n">
-        <v>2516.9204</v>
+        <v>2516.92</v>
       </c>
       <c r="CN253" t="n">
-        <v>2516.9334</v>
+        <v>2516.93</v>
       </c>
       <c r="CO253" t="n">
-        <v>1833.7227</v>
+        <v>1833.72</v>
       </c>
       <c r="CP253" t="n">
-        <v>1611.4091</v>
+        <v>1611.41</v>
       </c>
     </row>
     <row r="254">
@@ -39188,16 +39188,16 @@
         <v>0</v>
       </c>
       <c r="BD254" t="n">
-        <v>1163.7111</v>
+        <v>1163.7</v>
       </c>
       <c r="BE254" t="n">
-        <v>801.1724</v>
+        <v>801.17</v>
       </c>
       <c r="BF254" t="n">
-        <v>309.0645</v>
+        <v>309.06</v>
       </c>
       <c r="BG254" t="n">
-        <v>222.3092</v>
+        <v>222.31</v>
       </c>
       <c r="BH254" t="inlineStr"/>
       <c r="BI254" t="inlineStr"/>
@@ -39231,16 +39231,16 @@
       <c r="CK254" t="inlineStr"/>
       <c r="CL254" t="inlineStr"/>
       <c r="CM254" t="n">
-        <v>226.1399</v>
+        <v>226.14</v>
       </c>
       <c r="CN254" t="n">
-        <v>161.2239</v>
+        <v>161.22</v>
       </c>
       <c r="CO254" t="n">
-        <v>117.2414</v>
+        <v>117.24</v>
       </c>
       <c r="CP254" t="n">
-        <v>104.1266</v>
+        <v>104.13</v>
       </c>
     </row>
     <row r="255">
@@ -39400,13 +39400,13 @@
         <v>0</v>
       </c>
       <c r="CN255" t="n">
-        <v>144.4806</v>
+        <v>144.48</v>
       </c>
       <c r="CO255" t="n">
-        <v>168.9658</v>
+        <v>168.97</v>
       </c>
       <c r="CP255" t="n">
-        <v>126.1739</v>
+        <v>126.17</v>
       </c>
     </row>
     <row r="256">
@@ -39662,16 +39662,16 @@
         <v>0</v>
       </c>
       <c r="BD257" t="n">
-        <v>2.3169</v>
+        <v>2.32</v>
       </c>
       <c r="BE257" t="n">
-        <v>347.5725</v>
+        <v>347.57</v>
       </c>
       <c r="BF257" t="n">
-        <v>124.7023</v>
+        <v>124.7</v>
       </c>
       <c r="BG257" t="n">
-        <v>86.33839999999999</v>
+        <v>86.34</v>
       </c>
       <c r="BH257" t="inlineStr"/>
       <c r="BI257" t="inlineStr"/>
@@ -39705,16 +39705,16 @@
       <c r="CK257" t="inlineStr"/>
       <c r="CL257" t="inlineStr"/>
       <c r="CM257" t="n">
-        <v>115.3834</v>
+        <v>115.38</v>
       </c>
       <c r="CN257" t="n">
-        <v>120.0638</v>
+        <v>120.06</v>
       </c>
       <c r="CO257" t="n">
-        <v>112.4065</v>
+        <v>112.41</v>
       </c>
       <c r="CP257" t="n">
-        <v>96.60339999999999</v>
+        <v>96.59999999999999</v>
       </c>
     </row>
     <row r="258">
@@ -40542,10 +40542,10 @@
       <c r="BH262" t="inlineStr"/>
       <c r="BI262" t="inlineStr"/>
       <c r="BJ262" t="n">
-        <v>89.27770000000001</v>
+        <v>89.28</v>
       </c>
       <c r="BK262" t="n">
-        <v>95.839</v>
+        <v>95.84</v>
       </c>
       <c r="BL262" t="n">
         <v>85.98</v>
@@ -40577,16 +40577,16 @@
       <c r="CK262" t="inlineStr"/>
       <c r="CL262" t="inlineStr"/>
       <c r="CM262" t="n">
-        <v>197.0112</v>
+        <v>197.01</v>
       </c>
       <c r="CN262" t="n">
-        <v>205.8924</v>
+        <v>205.89</v>
       </c>
       <c r="CO262" t="n">
-        <v>175.9873</v>
+        <v>175.99</v>
       </c>
       <c r="CP262" t="n">
-        <v>190.2007</v>
+        <v>190.2</v>
       </c>
     </row>
     <row r="263">
@@ -40721,13 +40721,13 @@
       <c r="BK263" t="inlineStr"/>
       <c r="BL263" t="inlineStr"/>
       <c r="BM263" t="n">
-        <v>136.2488</v>
+        <v>136.25</v>
       </c>
       <c r="BN263" t="n">
-        <v>131.7333</v>
+        <v>131.73</v>
       </c>
       <c r="BO263" t="n">
-        <v>128.158</v>
+        <v>128.16</v>
       </c>
       <c r="BP263" t="inlineStr"/>
       <c r="BQ263" t="inlineStr"/>
@@ -40753,16 +40753,16 @@
       <c r="CK263" t="inlineStr"/>
       <c r="CL263" t="inlineStr"/>
       <c r="CM263" t="n">
-        <v>153.6441</v>
+        <v>153.64</v>
       </c>
       <c r="CN263" t="n">
-        <v>123.9354</v>
+        <v>123.94</v>
       </c>
       <c r="CO263" t="n">
-        <v>86.30670000000001</v>
+        <v>86.31</v>
       </c>
       <c r="CP263" t="n">
-        <v>169.894</v>
+        <v>169.89</v>
       </c>
     </row>
     <row r="264">
@@ -40866,16 +40866,16 @@
         <v>2006</v>
       </c>
       <c r="BB264" t="n">
-        <v>687.8371000000001</v>
+        <v>687.84</v>
       </c>
       <c r="BC264" t="n">
-        <v>414.0196</v>
+        <v>414.02</v>
       </c>
       <c r="BD264" t="n">
-        <v>883.9822</v>
+        <v>883.98</v>
       </c>
       <c r="BE264" t="n">
-        <v>277.1899</v>
+        <v>277.19</v>
       </c>
       <c r="BF264" t="inlineStr"/>
       <c r="BG264" t="inlineStr"/>
@@ -40911,16 +40911,16 @@
       <c r="CK264" t="inlineStr"/>
       <c r="CL264" t="inlineStr"/>
       <c r="CM264" t="n">
-        <v>277.1899</v>
+        <v>277.19</v>
       </c>
       <c r="CN264" t="n">
-        <v>231.1456</v>
+        <v>231.15</v>
       </c>
       <c r="CO264" t="n">
-        <v>227.0189</v>
+        <v>227.02</v>
       </c>
       <c r="CP264" t="n">
-        <v>139.3756</v>
+        <v>139.38</v>
       </c>
     </row>
     <row r="265">
@@ -41186,19 +41186,19 @@
       <c r="BD266" t="inlineStr"/>
       <c r="BE266" t="inlineStr"/>
       <c r="BF266" t="n">
-        <v>62.5274</v>
+        <v>62.53</v>
       </c>
       <c r="BG266" t="n">
-        <v>57.2501</v>
+        <v>57.25</v>
       </c>
       <c r="BH266" t="n">
-        <v>126.4626</v>
+        <v>126.46</v>
       </c>
       <c r="BI266" t="n">
-        <v>280.4459</v>
+        <v>280.45</v>
       </c>
       <c r="BJ266" t="n">
-        <v>165.2374</v>
+        <v>165.24</v>
       </c>
       <c r="BK266" t="inlineStr"/>
       <c r="BL266" t="inlineStr"/>
@@ -41229,16 +41229,16 @@
       <c r="CK266" t="inlineStr"/>
       <c r="CL266" t="inlineStr"/>
       <c r="CM266" t="n">
-        <v>150.7401</v>
+        <v>150.74</v>
       </c>
       <c r="CN266" t="n">
-        <v>162.868</v>
+        <v>162.87</v>
       </c>
       <c r="CO266" t="n">
-        <v>152.6307</v>
+        <v>152.63</v>
       </c>
       <c r="CP266" t="n">
-        <v>139.7682</v>
+        <v>139.77</v>
       </c>
     </row>
     <row r="267">
@@ -41356,19 +41356,19 @@
       <c r="BD267" t="inlineStr"/>
       <c r="BE267" t="inlineStr"/>
       <c r="BF267" t="n">
-        <v>663.8512000000001</v>
+        <v>663.85</v>
       </c>
       <c r="BG267" t="n">
-        <v>341.7916999999999</v>
+        <v>341.79</v>
       </c>
       <c r="BH267" t="n">
-        <v>341.9413999999999</v>
+        <v>341.94</v>
       </c>
       <c r="BI267" t="n">
-        <v>342.0137999999999</v>
+        <v>342.01</v>
       </c>
       <c r="BJ267" t="n">
-        <v>1056.2626</v>
+        <v>1056.26</v>
       </c>
       <c r="BK267" t="inlineStr"/>
       <c r="BL267" t="inlineStr"/>
@@ -41399,16 +41399,16 @@
       <c r="CK267" t="inlineStr"/>
       <c r="CL267" t="inlineStr"/>
       <c r="CM267" t="n">
-        <v>1056.4699</v>
+        <v>1056.47</v>
       </c>
       <c r="CN267" t="n">
-        <v>1251.0251</v>
+        <v>1251.03</v>
       </c>
       <c r="CO267" t="n">
-        <v>109.7551</v>
+        <v>109.76</v>
       </c>
       <c r="CP267" t="n">
-        <v>1294.8031</v>
+        <v>1294.8</v>
       </c>
     </row>
     <row r="268">
@@ -41514,19 +41514,19 @@
         <v>2005</v>
       </c>
       <c r="BB268" t="n">
-        <v>4225.2176</v>
+        <v>4225.22</v>
       </c>
       <c r="BC268" t="n">
-        <v>3983.7536</v>
+        <v>3983.75</v>
       </c>
       <c r="BD268" t="n">
-        <v>4008.8248</v>
+        <v>4008.82</v>
       </c>
       <c r="BE268" t="n">
-        <v>4027.7778</v>
+        <v>4027.78</v>
       </c>
       <c r="BF268" t="n">
-        <v>4008.028600000001</v>
+        <v>4008.03</v>
       </c>
       <c r="BG268" t="inlineStr"/>
       <c r="BH268" t="inlineStr"/>
@@ -41561,16 +41561,16 @@
       <c r="CK268" t="inlineStr"/>
       <c r="CL268" t="inlineStr"/>
       <c r="CM268" t="n">
-        <v>7.179399999999999</v>
+        <v>7.18</v>
       </c>
       <c r="CN268" t="n">
-        <v>3973.147</v>
+        <v>3973.15</v>
       </c>
       <c r="CO268" t="n">
-        <v>3972.3523</v>
+        <v>3972.35</v>
       </c>
       <c r="CP268" t="n">
-        <v>4023.1173</v>
+        <v>4023.12</v>
       </c>
     </row>
     <row r="269">
@@ -41842,16 +41842,16 @@
         <v>2003</v>
       </c>
       <c r="BB270" t="n">
-        <v>0.0001</v>
+        <v>0</v>
       </c>
       <c r="BC270" t="n">
-        <v>264.8121</v>
+        <v>264.81</v>
       </c>
       <c r="BD270" t="n">
-        <v>916409.7336999999</v>
+        <v>916409.73</v>
       </c>
       <c r="BE270" t="n">
-        <v>162045.5936</v>
+        <v>162045.59</v>
       </c>
       <c r="BF270" t="inlineStr"/>
       <c r="BG270" t="inlineStr"/>
@@ -41887,16 +41887,16 @@
       <c r="CK270" t="inlineStr"/>
       <c r="CL270" t="inlineStr"/>
       <c r="CM270" t="n">
-        <v>162045.5936</v>
+        <v>162045.59</v>
       </c>
       <c r="CN270" t="n">
-        <v>40.0417</v>
+        <v>40.04</v>
       </c>
       <c r="CO270" t="n">
-        <v>63.641</v>
+        <v>63.64</v>
       </c>
       <c r="CP270" t="n">
-        <v>9301.0129</v>
+        <v>9301.01</v>
       </c>
     </row>
     <row r="271">
@@ -42335,16 +42335,16 @@
       <c r="CK273" t="inlineStr"/>
       <c r="CL273" t="inlineStr"/>
       <c r="CM273" t="n">
-        <v>6437.721300000001</v>
+        <v>6437.72</v>
       </c>
       <c r="CN273" t="n">
-        <v>6437.576900000001</v>
+        <v>6437.58</v>
       </c>
       <c r="CO273" t="n">
-        <v>6372.864</v>
+        <v>6372.86</v>
       </c>
       <c r="CP273" t="n">
-        <v>1314.5037</v>
+        <v>1314.5</v>
       </c>
     </row>
     <row r="274">
@@ -43488,19 +43488,19 @@
         <v>2007</v>
       </c>
       <c r="BB280" t="n">
-        <v>2596.8404</v>
+        <v>2596.84</v>
       </c>
       <c r="BC280" t="n">
-        <v>2573.2574</v>
+        <v>2573.26</v>
       </c>
       <c r="BD280" t="n">
-        <v>2707.1801</v>
+        <v>2707.18</v>
       </c>
       <c r="BE280" t="n">
-        <v>2709.4211</v>
+        <v>2709.42</v>
       </c>
       <c r="BF280" t="n">
-        <v>2654.3441</v>
+        <v>2654.34</v>
       </c>
       <c r="BG280" t="inlineStr"/>
       <c r="BH280" t="inlineStr"/>
@@ -43535,16 +43535,16 @@
       <c r="CK280" t="inlineStr"/>
       <c r="CL280" t="inlineStr"/>
       <c r="CM280" t="n">
-        <v>2704.8581</v>
+        <v>2704.86</v>
       </c>
       <c r="CN280" t="n">
-        <v>2704.8949</v>
+        <v>2704.89</v>
       </c>
       <c r="CO280" t="n">
-        <v>2689.9132</v>
+        <v>2689.91</v>
       </c>
       <c r="CP280" t="n">
-        <v>2690.7867</v>
+        <v>2690.79</v>
       </c>
     </row>
     <row r="281">
@@ -43650,19 +43650,19 @@
         <v>2007</v>
       </c>
       <c r="BB281" t="n">
-        <v>93.66290000000001</v>
+        <v>93.66</v>
       </c>
       <c r="BC281" t="n">
-        <v>78.50590000000001</v>
+        <v>78.51000000000001</v>
       </c>
       <c r="BD281" t="n">
-        <v>74.6955</v>
+        <v>74.7</v>
       </c>
       <c r="BE281" t="n">
-        <v>75.0941</v>
+        <v>75.09</v>
       </c>
       <c r="BF281" t="n">
-        <v>78.33799999999999</v>
+        <v>78.34</v>
       </c>
       <c r="BG281" t="inlineStr"/>
       <c r="BH281" t="inlineStr"/>
@@ -43697,16 +43697,16 @@
       <c r="CK281" t="inlineStr"/>
       <c r="CL281" t="inlineStr"/>
       <c r="CM281" t="n">
-        <v>74.39790000000001</v>
+        <v>74.40000000000001</v>
       </c>
       <c r="CN281" t="n">
-        <v>66.74460000000001</v>
+        <v>66.73999999999999</v>
       </c>
       <c r="CO281" t="n">
-        <v>63.2785</v>
+        <v>63.28</v>
       </c>
       <c r="CP281" t="n">
-        <v>54.01090000000001</v>
+        <v>54.01</v>
       </c>
     </row>
     <row r="282">
@@ -43812,19 +43812,19 @@
         <v>2007</v>
       </c>
       <c r="BB282" t="n">
-        <v>92.1062</v>
+        <v>92.11</v>
       </c>
       <c r="BC282" t="n">
-        <v>104.5992</v>
+        <v>104.6</v>
       </c>
       <c r="BD282" t="n">
-        <v>101.3696</v>
+        <v>101.37</v>
       </c>
       <c r="BE282" t="n">
-        <v>116.5759</v>
+        <v>116.58</v>
       </c>
       <c r="BF282" t="n">
-        <v>108.6637</v>
+        <v>108.66</v>
       </c>
       <c r="BG282" t="inlineStr"/>
       <c r="BH282" t="inlineStr"/>
@@ -43859,16 +43859,16 @@
       <c r="CK282" t="inlineStr"/>
       <c r="CL282" t="inlineStr"/>
       <c r="CM282" t="n">
-        <v>149.8387</v>
+        <v>149.84</v>
       </c>
       <c r="CN282" t="n">
-        <v>122.2124</v>
+        <v>122.21</v>
       </c>
       <c r="CO282" t="n">
-        <v>116.9921</v>
+        <v>116.99</v>
       </c>
       <c r="CP282" t="n">
-        <v>110.2906</v>
+        <v>110.29</v>
       </c>
     </row>
     <row r="283">
@@ -43974,19 +43974,19 @@
         <v>2007</v>
       </c>
       <c r="BB283" t="n">
-        <v>4.7278</v>
+        <v>4.73</v>
       </c>
       <c r="BC283" t="n">
-        <v>4.678199999999999</v>
+        <v>4.68</v>
       </c>
       <c r="BD283" t="n">
-        <v>5.1791</v>
+        <v>5.18</v>
       </c>
       <c r="BE283" t="n">
-        <v>6.434299999999999</v>
+        <v>6.43</v>
       </c>
       <c r="BF283" t="n">
-        <v>64.57859999999999</v>
+        <v>64.58</v>
       </c>
       <c r="BG283" t="inlineStr"/>
       <c r="BH283" t="inlineStr"/>
@@ -44021,16 +44021,16 @@
       <c r="CK283" t="inlineStr"/>
       <c r="CL283" t="inlineStr"/>
       <c r="CM283" t="n">
-        <v>28.0552</v>
+        <v>28.06</v>
       </c>
       <c r="CN283" t="n">
-        <v>62.65840000000001</v>
+        <v>62.66</v>
       </c>
       <c r="CO283" t="n">
-        <v>2.2427</v>
+        <v>2.24</v>
       </c>
       <c r="CP283" t="n">
-        <v>2.2375</v>
+        <v>2.24</v>
       </c>
     </row>
     <row r="284">
@@ -44703,25 +44703,25 @@
       </c>
       <c r="BB288" t="inlineStr"/>
       <c r="BC288" t="n">
-        <v>1827.2834</v>
+        <v>1827.28</v>
       </c>
       <c r="BD288" t="n">
-        <v>1827.2391</v>
+        <v>1827.24</v>
       </c>
       <c r="BE288" t="n">
-        <v>1812.3049</v>
+        <v>1812.3</v>
       </c>
       <c r="BF288" t="n">
-        <v>1337.5224</v>
+        <v>1337.52</v>
       </c>
       <c r="BG288" t="n">
-        <v>257.0056</v>
+        <v>257.01</v>
       </c>
       <c r="BH288" t="n">
-        <v>257.9087</v>
+        <v>257.91</v>
       </c>
       <c r="BI288" t="n">
-        <v>54.6182</v>
+        <v>54.62</v>
       </c>
       <c r="BJ288" t="inlineStr"/>
       <c r="BK288" t="inlineStr"/>
@@ -44753,16 +44753,16 @@
       <c r="CK288" t="inlineStr"/>
       <c r="CL288" t="inlineStr"/>
       <c r="CM288" t="n">
-        <v>87.07140000000001</v>
+        <v>87.06999999999999</v>
       </c>
       <c r="CN288" t="n">
-        <v>252.7047</v>
+        <v>252.7</v>
       </c>
       <c r="CO288" t="n">
-        <v>792.5236999999998</v>
+        <v>792.52</v>
       </c>
       <c r="CP288" t="n">
-        <v>305.3924</v>
+        <v>305.39</v>
       </c>
     </row>
     <row r="289">
@@ -45160,22 +45160,22 @@
         <v>2010</v>
       </c>
       <c r="BB291" t="n">
-        <v>429.3869</v>
+        <v>429.39</v>
       </c>
       <c r="BC291" t="n">
-        <v>509.9654</v>
+        <v>509.97</v>
       </c>
       <c r="BD291" t="n">
-        <v>555.5272</v>
+        <v>555.53</v>
       </c>
       <c r="BE291" t="n">
-        <v>580.9227000000001</v>
+        <v>580.92</v>
       </c>
       <c r="BF291" t="n">
-        <v>451.2565</v>
+        <v>451.26</v>
       </c>
       <c r="BG291" t="n">
-        <v>561.6615</v>
+        <v>561.66</v>
       </c>
       <c r="BH291" t="inlineStr"/>
       <c r="BI291" t="inlineStr"/>
@@ -45209,16 +45209,16 @@
       <c r="CK291" t="inlineStr"/>
       <c r="CL291" t="inlineStr"/>
       <c r="CM291" t="n">
-        <v>502.5194</v>
+        <v>502.52</v>
       </c>
       <c r="CN291" t="n">
-        <v>548.3257</v>
+        <v>548.33</v>
       </c>
       <c r="CO291" t="n">
-        <v>492.4741</v>
+        <v>492.47</v>
       </c>
       <c r="CP291" t="n">
-        <v>418.1197</v>
+        <v>418.12</v>
       </c>
     </row>
     <row r="292">
@@ -45326,22 +45326,22 @@
         <v>2010</v>
       </c>
       <c r="BB292" t="n">
-        <v>79.1602</v>
+        <v>79.16</v>
       </c>
       <c r="BC292" t="n">
-        <v>62.5477</v>
+        <v>62.55</v>
       </c>
       <c r="BD292" t="n">
-        <v>32.9716</v>
+        <v>32.97</v>
       </c>
       <c r="BE292" t="n">
-        <v>28.6115</v>
+        <v>28.61</v>
       </c>
       <c r="BF292" t="n">
-        <v>26.8337</v>
+        <v>26.83</v>
       </c>
       <c r="BG292" t="n">
-        <v>23.3364</v>
+        <v>23.34</v>
       </c>
       <c r="BH292" t="inlineStr"/>
       <c r="BI292" t="inlineStr"/>
@@ -45375,16 +45375,16 @@
       <c r="CK292" t="inlineStr"/>
       <c r="CL292" t="inlineStr"/>
       <c r="CM292" t="n">
-        <v>42.8431</v>
+        <v>42.84</v>
       </c>
       <c r="CN292" t="n">
-        <v>39.5805</v>
+        <v>39.58</v>
       </c>
       <c r="CO292" t="n">
-        <v>38.0499</v>
+        <v>38.05</v>
       </c>
       <c r="CP292" t="n">
-        <v>39.4791</v>
+        <v>39.48</v>
       </c>
     </row>
     <row r="293">

</xml_diff>

<commit_message>
Updated 04 and 05 and did some experiments with cartel_df_sh
</commit_message>
<xml_diff>
--- a/transformed_data/cartel_networks/test222.xlsx
+++ b/transformed_data/cartel_networks/test222.xlsx
@@ -1555,9 +1555,7 @@
       <c r="CM5" t="inlineStr"/>
       <c r="CN5" t="inlineStr"/>
       <c r="CO5" t="inlineStr"/>
-      <c r="CP5" t="n">
-        <v>663.85</v>
-      </c>
+      <c r="CP5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -12802,18 +12800,10 @@
         <v>2004</v>
       </c>
       <c r="BB83" t="inlineStr"/>
-      <c r="BC83" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD83" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE83" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF83" t="n">
-        <v>0</v>
-      </c>
+      <c r="BC83" t="inlineStr"/>
+      <c r="BD83" t="inlineStr"/>
+      <c r="BE83" t="inlineStr"/>
+      <c r="BF83" t="inlineStr"/>
       <c r="BG83" t="inlineStr"/>
       <c r="BH83" t="inlineStr"/>
       <c r="BI83" t="inlineStr"/>
@@ -12846,18 +12836,10 @@
       <c r="CJ83" t="inlineStr"/>
       <c r="CK83" t="inlineStr"/>
       <c r="CL83" t="inlineStr"/>
-      <c r="CM83" t="n">
-        <v>985.9299999999999</v>
-      </c>
-      <c r="CN83" t="n">
-        <v>966.8099999999999</v>
-      </c>
-      <c r="CO83" t="n">
-        <v>964.91</v>
-      </c>
-      <c r="CP83" t="n">
-        <v>976.14</v>
-      </c>
+      <c r="CM83" t="inlineStr"/>
+      <c r="CN83" t="inlineStr"/>
+      <c r="CO83" t="inlineStr"/>
+      <c r="CP83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="n">
@@ -15016,9 +14998,7 @@
       <c r="BF98" t="inlineStr"/>
       <c r="BG98" t="inlineStr"/>
       <c r="BH98" t="inlineStr"/>
-      <c r="BI98" t="n">
-        <v>48.8</v>
-      </c>
+      <c r="BI98" t="inlineStr"/>
       <c r="BJ98" t="inlineStr"/>
       <c r="BK98" t="inlineStr"/>
       <c r="BL98" t="inlineStr"/>
@@ -15048,18 +15028,10 @@
       <c r="CJ98" t="inlineStr"/>
       <c r="CK98" t="inlineStr"/>
       <c r="CL98" t="inlineStr"/>
-      <c r="CM98" t="n">
-        <v>186.41</v>
-      </c>
-      <c r="CN98" t="n">
-        <v>196.13</v>
-      </c>
-      <c r="CO98" t="n">
-        <v>4.77</v>
-      </c>
-      <c r="CP98" t="n">
-        <v>3.52</v>
-      </c>
+      <c r="CM98" t="inlineStr"/>
+      <c r="CN98" t="inlineStr"/>
+      <c r="CO98" t="inlineStr"/>
+      <c r="CP98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="n">
@@ -17697,9 +17669,7 @@
       <c r="BO116" t="inlineStr"/>
       <c r="BP116" t="inlineStr"/>
       <c r="BQ116" t="inlineStr"/>
-      <c r="BR116" t="n">
-        <v>48.8</v>
-      </c>
+      <c r="BR116" t="inlineStr"/>
       <c r="BS116" t="inlineStr"/>
       <c r="BT116" t="inlineStr"/>
       <c r="BU116" t="inlineStr"/>
@@ -17720,18 +17690,10 @@
       <c r="CJ116" t="inlineStr"/>
       <c r="CK116" t="inlineStr"/>
       <c r="CL116" t="inlineStr"/>
-      <c r="CM116" t="n">
-        <v>186.41</v>
-      </c>
-      <c r="CN116" t="n">
-        <v>196.13</v>
-      </c>
-      <c r="CO116" t="n">
-        <v>4.77</v>
-      </c>
-      <c r="CP116" t="n">
-        <v>3.52</v>
-      </c>
+      <c r="CM116" t="inlineStr"/>
+      <c r="CN116" t="inlineStr"/>
+      <c r="CO116" t="inlineStr"/>
+      <c r="CP116" t="inlineStr"/>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -17984,18 +17946,10 @@
         <v>2004</v>
       </c>
       <c r="BB118" t="inlineStr"/>
-      <c r="BC118" t="n">
-        <v>12.94</v>
-      </c>
-      <c r="BD118" t="n">
-        <v>62.03</v>
-      </c>
-      <c r="BE118" t="n">
-        <v>80.12</v>
-      </c>
-      <c r="BF118" t="n">
-        <v>575.45</v>
-      </c>
+      <c r="BC118" t="inlineStr"/>
+      <c r="BD118" t="inlineStr"/>
+      <c r="BE118" t="inlineStr"/>
+      <c r="BF118" t="inlineStr"/>
       <c r="BG118" t="inlineStr"/>
       <c r="BH118" t="inlineStr"/>
       <c r="BI118" t="inlineStr"/>
@@ -18028,18 +17982,10 @@
       <c r="CJ118" t="inlineStr"/>
       <c r="CK118" t="inlineStr"/>
       <c r="CL118" t="inlineStr"/>
-      <c r="CM118" t="n">
-        <v>219.38</v>
-      </c>
-      <c r="CN118" t="n">
-        <v>267.14</v>
-      </c>
-      <c r="CO118" t="n">
-        <v>196.39</v>
-      </c>
-      <c r="CP118" t="n">
-        <v>201.03</v>
-      </c>
+      <c r="CM118" t="inlineStr"/>
+      <c r="CN118" t="inlineStr"/>
+      <c r="CO118" t="inlineStr"/>
+      <c r="CP118" t="inlineStr"/>
     </row>
     <row r="119">
       <c r="A119" t="n">
@@ -18589,15 +18535,9 @@
       </c>
       <c r="BB122" t="inlineStr"/>
       <c r="BC122" t="inlineStr"/>
-      <c r="BD122" t="n">
-        <v>89.28</v>
-      </c>
-      <c r="BE122" t="n">
-        <v>95.84</v>
-      </c>
-      <c r="BF122" t="n">
-        <v>85.98</v>
-      </c>
+      <c r="BD122" t="inlineStr"/>
+      <c r="BE122" t="inlineStr"/>
+      <c r="BF122" t="inlineStr"/>
       <c r="BG122" t="inlineStr"/>
       <c r="BH122" t="inlineStr"/>
       <c r="BI122" t="inlineStr"/>
@@ -18630,18 +18570,10 @@
       <c r="CJ122" t="inlineStr"/>
       <c r="CK122" t="inlineStr"/>
       <c r="CL122" t="inlineStr"/>
-      <c r="CM122" t="n">
-        <v>197.01</v>
-      </c>
-      <c r="CN122" t="n">
-        <v>205.89</v>
-      </c>
-      <c r="CO122" t="n">
-        <v>175.99</v>
-      </c>
-      <c r="CP122" t="n">
-        <v>190.2</v>
-      </c>
+      <c r="CM122" t="inlineStr"/>
+      <c r="CN122" t="inlineStr"/>
+      <c r="CO122" t="inlineStr"/>
+      <c r="CP122" t="inlineStr"/>
     </row>
     <row r="123">
       <c r="A123" t="n">
@@ -19231,15 +19163,9 @@
       <c r="BK126" t="inlineStr"/>
       <c r="BL126" t="inlineStr"/>
       <c r="BM126" t="inlineStr"/>
-      <c r="BN126" t="n">
-        <v>0</v>
-      </c>
-      <c r="BO126" t="n">
-        <v>264.81</v>
-      </c>
-      <c r="BP126" t="n">
-        <v>916409.73</v>
-      </c>
+      <c r="BN126" t="inlineStr"/>
+      <c r="BO126" t="inlineStr"/>
+      <c r="BP126" t="inlineStr"/>
       <c r="BQ126" t="inlineStr"/>
       <c r="BR126" t="inlineStr"/>
       <c r="BS126" t="inlineStr"/>
@@ -19262,18 +19188,10 @@
       <c r="CJ126" t="inlineStr"/>
       <c r="CK126" t="inlineStr"/>
       <c r="CL126" t="inlineStr"/>
-      <c r="CM126" t="n">
-        <v>162045.59</v>
-      </c>
-      <c r="CN126" t="n">
-        <v>40.04</v>
-      </c>
-      <c r="CO126" t="n">
-        <v>63.64</v>
-      </c>
-      <c r="CP126" t="n">
-        <v>9301.01</v>
-      </c>
+      <c r="CM126" t="inlineStr"/>
+      <c r="CN126" t="inlineStr"/>
+      <c r="CO126" t="inlineStr"/>
+      <c r="CP126" t="inlineStr"/>
     </row>
     <row r="127">
       <c r="A127" t="n">
@@ -19403,15 +19321,9 @@
       <c r="BI127" t="inlineStr"/>
       <c r="BJ127" t="inlineStr"/>
       <c r="BK127" t="inlineStr"/>
-      <c r="BL127" t="n">
-        <v>136.25</v>
-      </c>
-      <c r="BM127" t="n">
-        <v>131.73</v>
-      </c>
-      <c r="BN127" t="n">
-        <v>128.16</v>
-      </c>
+      <c r="BL127" t="inlineStr"/>
+      <c r="BM127" t="inlineStr"/>
+      <c r="BN127" t="inlineStr"/>
       <c r="BO127" t="inlineStr"/>
       <c r="BP127" t="inlineStr"/>
       <c r="BQ127" t="inlineStr"/>
@@ -19436,18 +19348,10 @@
       <c r="CJ127" t="inlineStr"/>
       <c r="CK127" t="inlineStr"/>
       <c r="CL127" t="inlineStr"/>
-      <c r="CM127" t="n">
-        <v>153.64</v>
-      </c>
-      <c r="CN127" t="n">
-        <v>123.94</v>
-      </c>
-      <c r="CO127" t="n">
-        <v>86.31</v>
-      </c>
-      <c r="CP127" t="n">
-        <v>169.89</v>
-      </c>
+      <c r="CM127" t="inlineStr"/>
+      <c r="CN127" t="inlineStr"/>
+      <c r="CO127" t="inlineStr"/>
+      <c r="CP127" t="inlineStr"/>
     </row>
     <row r="128">
       <c r="A128" t="n">
@@ -21655,18 +21559,10 @@
       <c r="BA142" t="n">
         <v>2004</v>
       </c>
-      <c r="BB142" t="n">
-        <v>2498.4</v>
-      </c>
-      <c r="BC142" t="n">
-        <v>2498.55</v>
-      </c>
-      <c r="BD142" t="n">
-        <v>2699.15</v>
-      </c>
-      <c r="BE142" t="n">
-        <v>2686.5</v>
-      </c>
+      <c r="BB142" t="inlineStr"/>
+      <c r="BC142" t="inlineStr"/>
+      <c r="BD142" t="inlineStr"/>
+      <c r="BE142" t="inlineStr"/>
       <c r="BF142" t="inlineStr"/>
       <c r="BG142" t="inlineStr"/>
       <c r="BH142" t="inlineStr"/>
@@ -21700,18 +21596,10 @@
       <c r="CJ142" t="inlineStr"/>
       <c r="CK142" t="inlineStr"/>
       <c r="CL142" t="inlineStr"/>
-      <c r="CM142" t="n">
-        <v>2685.72</v>
-      </c>
-      <c r="CN142" t="n">
-        <v>2685.01</v>
-      </c>
-      <c r="CO142" t="n">
-        <v>2646.44</v>
-      </c>
-      <c r="CP142" t="n">
-        <v>2645.41</v>
-      </c>
+      <c r="CM142" t="inlineStr"/>
+      <c r="CN142" t="inlineStr"/>
+      <c r="CO142" t="inlineStr"/>
+      <c r="CP142" t="inlineStr"/>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -21813,18 +21701,10 @@
       <c r="BA143" t="n">
         <v>2004</v>
       </c>
-      <c r="BB143" t="n">
-        <v>14.32</v>
-      </c>
-      <c r="BC143" t="n">
-        <v>15.66</v>
-      </c>
-      <c r="BD143" t="n">
-        <v>42</v>
-      </c>
-      <c r="BE143" t="n">
-        <v>82.33</v>
-      </c>
+      <c r="BB143" t="inlineStr"/>
+      <c r="BC143" t="inlineStr"/>
+      <c r="BD143" t="inlineStr"/>
+      <c r="BE143" t="inlineStr"/>
       <c r="BF143" t="inlineStr"/>
       <c r="BG143" t="inlineStr"/>
       <c r="BH143" t="inlineStr"/>
@@ -21858,18 +21738,10 @@
       <c r="CJ143" t="inlineStr"/>
       <c r="CK143" t="inlineStr"/>
       <c r="CL143" t="inlineStr"/>
-      <c r="CM143" t="n">
-        <v>29.04</v>
-      </c>
-      <c r="CN143" t="n">
-        <v>22.62</v>
-      </c>
-      <c r="CO143" t="n">
-        <v>17.72</v>
-      </c>
-      <c r="CP143" t="n">
-        <v>15.28</v>
-      </c>
+      <c r="CM143" t="inlineStr"/>
+      <c r="CN143" t="inlineStr"/>
+      <c r="CO143" t="inlineStr"/>
+      <c r="CP143" t="inlineStr"/>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -21971,18 +21843,10 @@
       <c r="BA144" t="n">
         <v>2004</v>
       </c>
-      <c r="BB144" t="n">
-        <v>108.23</v>
-      </c>
-      <c r="BC144" t="n">
-        <v>118.76</v>
-      </c>
-      <c r="BD144" t="n">
-        <v>135.11</v>
-      </c>
-      <c r="BE144" t="n">
-        <v>96.3</v>
-      </c>
+      <c r="BB144" t="inlineStr"/>
+      <c r="BC144" t="inlineStr"/>
+      <c r="BD144" t="inlineStr"/>
+      <c r="BE144" t="inlineStr"/>
       <c r="BF144" t="inlineStr"/>
       <c r="BG144" t="inlineStr"/>
       <c r="BH144" t="inlineStr"/>
@@ -22016,18 +21880,10 @@
       <c r="CJ144" t="inlineStr"/>
       <c r="CK144" t="inlineStr"/>
       <c r="CL144" t="inlineStr"/>
-      <c r="CM144" t="n">
-        <v>100.18</v>
-      </c>
-      <c r="CN144" t="n">
-        <v>78.61</v>
-      </c>
-      <c r="CO144" t="n">
-        <v>90.25</v>
-      </c>
-      <c r="CP144" t="n">
-        <v>76.97</v>
-      </c>
+      <c r="CM144" t="inlineStr"/>
+      <c r="CN144" t="inlineStr"/>
+      <c r="CO144" t="inlineStr"/>
+      <c r="CP144" t="inlineStr"/>
     </row>
     <row r="145">
       <c r="A145" t="n">
@@ -22419,18 +22275,10 @@
       <c r="BA147" t="n">
         <v>2003</v>
       </c>
-      <c r="BB147" t="n">
-        <v>211.04</v>
-      </c>
-      <c r="BC147" t="n">
-        <v>221.72</v>
-      </c>
-      <c r="BD147" t="n">
-        <v>348.95</v>
-      </c>
-      <c r="BE147" t="n">
-        <v>276.17</v>
-      </c>
+      <c r="BB147" t="inlineStr"/>
+      <c r="BC147" t="inlineStr"/>
+      <c r="BD147" t="inlineStr"/>
+      <c r="BE147" t="inlineStr"/>
       <c r="BF147" t="inlineStr"/>
       <c r="BG147" t="inlineStr"/>
       <c r="BH147" t="inlineStr"/>
@@ -22464,18 +22312,10 @@
       <c r="CJ147" t="inlineStr"/>
       <c r="CK147" t="inlineStr"/>
       <c r="CL147" t="inlineStr"/>
-      <c r="CM147" t="n">
-        <v>276.17</v>
-      </c>
-      <c r="CN147" t="n">
-        <v>336.54</v>
-      </c>
-      <c r="CO147" t="n">
-        <v>274.64</v>
-      </c>
-      <c r="CP147" t="n">
-        <v>169.06</v>
-      </c>
+      <c r="CM147" t="inlineStr"/>
+      <c r="CN147" t="inlineStr"/>
+      <c r="CO147" t="inlineStr"/>
+      <c r="CP147" t="inlineStr"/>
     </row>
     <row r="148">
       <c r="A148" t="n">
@@ -22873,18 +22713,10 @@
       <c r="BA150" t="n">
         <v>2004</v>
       </c>
-      <c r="BB150" t="n">
-        <v>16.28</v>
-      </c>
-      <c r="BC150" t="n">
-        <v>8.050000000000001</v>
-      </c>
-      <c r="BD150" t="n">
-        <v>1.52</v>
-      </c>
-      <c r="BE150" t="n">
-        <v>2.17</v>
-      </c>
+      <c r="BB150" t="inlineStr"/>
+      <c r="BC150" t="inlineStr"/>
+      <c r="BD150" t="inlineStr"/>
+      <c r="BE150" t="inlineStr"/>
       <c r="BF150" t="inlineStr"/>
       <c r="BG150" t="inlineStr"/>
       <c r="BH150" t="inlineStr"/>
@@ -22918,18 +22750,10 @@
       <c r="CJ150" t="inlineStr"/>
       <c r="CK150" t="inlineStr"/>
       <c r="CL150" t="inlineStr"/>
-      <c r="CM150" t="n">
-        <v>2.17</v>
-      </c>
-      <c r="CN150" t="n">
-        <v>21.22</v>
-      </c>
-      <c r="CO150" t="n">
-        <v>11.93</v>
-      </c>
-      <c r="CP150" t="n">
-        <v>14.21</v>
-      </c>
+      <c r="CM150" t="inlineStr"/>
+      <c r="CN150" t="inlineStr"/>
+      <c r="CO150" t="inlineStr"/>
+      <c r="CP150" t="inlineStr"/>
     </row>
     <row r="151">
       <c r="A151" t="n">
@@ -24379,12 +24203,8 @@
       <c r="BE160" t="inlineStr"/>
       <c r="BF160" t="inlineStr"/>
       <c r="BG160" t="inlineStr"/>
-      <c r="BH160" t="n">
-        <v>48.8</v>
-      </c>
-      <c r="BI160" t="n">
-        <v>186.41</v>
-      </c>
+      <c r="BH160" t="inlineStr"/>
+      <c r="BI160" t="inlineStr"/>
       <c r="BJ160" t="inlineStr"/>
       <c r="BK160" t="inlineStr"/>
       <c r="BL160" t="inlineStr"/>
@@ -24414,18 +24234,10 @@
       <c r="CJ160" t="inlineStr"/>
       <c r="CK160" t="inlineStr"/>
       <c r="CL160" t="inlineStr"/>
-      <c r="CM160" t="n">
-        <v>196.13</v>
-      </c>
-      <c r="CN160" t="n">
-        <v>4.77</v>
-      </c>
-      <c r="CO160" t="n">
-        <v>3.52</v>
-      </c>
-      <c r="CP160" t="n">
-        <v>31.49</v>
-      </c>
+      <c r="CM160" t="inlineStr"/>
+      <c r="CN160" t="inlineStr"/>
+      <c r="CO160" t="inlineStr"/>
+      <c r="CP160" t="inlineStr"/>
     </row>
     <row r="161">
       <c r="A161" t="n">
@@ -25242,12 +25054,8 @@
       <c r="BB166" t="inlineStr"/>
       <c r="BC166" t="inlineStr"/>
       <c r="BD166" t="inlineStr"/>
-      <c r="BE166" t="n">
-        <v>2.77</v>
-      </c>
-      <c r="BF166" t="n">
-        <v>12.17</v>
-      </c>
+      <c r="BE166" t="inlineStr"/>
+      <c r="BF166" t="inlineStr"/>
       <c r="BG166" t="inlineStr"/>
       <c r="BH166" t="inlineStr"/>
       <c r="BI166" t="inlineStr"/>
@@ -25280,18 +25088,10 @@
       <c r="CJ166" t="inlineStr"/>
       <c r="CK166" t="inlineStr"/>
       <c r="CL166" t="inlineStr"/>
-      <c r="CM166" t="n">
-        <v>4.61</v>
-      </c>
-      <c r="CN166" t="n">
-        <v>2.08</v>
-      </c>
-      <c r="CO166" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="CP166" t="n">
-        <v>0</v>
-      </c>
+      <c r="CM166" t="inlineStr"/>
+      <c r="CN166" t="inlineStr"/>
+      <c r="CO166" t="inlineStr"/>
+      <c r="CP166" t="inlineStr"/>
     </row>
     <row r="167">
       <c r="A167" t="n">
@@ -25397,24 +25197,12 @@
       <c r="BA167" t="n">
         <v>2006</v>
       </c>
-      <c r="BB167" t="n">
-        <v>663.85</v>
-      </c>
-      <c r="BC167" t="n">
-        <v>341.79</v>
-      </c>
-      <c r="BD167" t="n">
-        <v>341.94</v>
-      </c>
-      <c r="BE167" t="n">
-        <v>342.01</v>
-      </c>
-      <c r="BF167" t="n">
-        <v>1056.26</v>
-      </c>
-      <c r="BG167" t="n">
-        <v>1056.47</v>
-      </c>
+      <c r="BB167" t="inlineStr"/>
+      <c r="BC167" t="inlineStr"/>
+      <c r="BD167" t="inlineStr"/>
+      <c r="BE167" t="inlineStr"/>
+      <c r="BF167" t="inlineStr"/>
+      <c r="BG167" t="inlineStr"/>
       <c r="BH167" t="inlineStr"/>
       <c r="BI167" t="inlineStr"/>
       <c r="BJ167" t="inlineStr"/>
@@ -25446,18 +25234,10 @@
       <c r="CJ167" t="inlineStr"/>
       <c r="CK167" t="inlineStr"/>
       <c r="CL167" t="inlineStr"/>
-      <c r="CM167" t="n">
-        <v>1251.03</v>
-      </c>
-      <c r="CN167" t="n">
-        <v>109.76</v>
-      </c>
-      <c r="CO167" t="n">
-        <v>1294.8</v>
-      </c>
-      <c r="CP167" t="n">
-        <v>124.96</v>
-      </c>
+      <c r="CM167" t="inlineStr"/>
+      <c r="CN167" t="inlineStr"/>
+      <c r="CO167" t="inlineStr"/>
+      <c r="CP167" t="inlineStr"/>
     </row>
     <row r="168">
       <c r="A168" t="n">
@@ -25569,24 +25349,12 @@
       </c>
       <c r="BB168" t="inlineStr"/>
       <c r="BC168" t="inlineStr"/>
-      <c r="BD168" t="n">
-        <v>111.88</v>
-      </c>
-      <c r="BE168" t="n">
-        <v>122.69</v>
-      </c>
-      <c r="BF168" t="n">
-        <v>131.08</v>
-      </c>
-      <c r="BG168" t="n">
-        <v>119.38</v>
-      </c>
-      <c r="BH168" t="n">
-        <v>73.20999999999999</v>
-      </c>
-      <c r="BI168" t="n">
-        <v>64.14</v>
-      </c>
+      <c r="BD168" t="inlineStr"/>
+      <c r="BE168" t="inlineStr"/>
+      <c r="BF168" t="inlineStr"/>
+      <c r="BG168" t="inlineStr"/>
+      <c r="BH168" t="inlineStr"/>
+      <c r="BI168" t="inlineStr"/>
       <c r="BJ168" t="inlineStr"/>
       <c r="BK168" t="inlineStr"/>
       <c r="BL168" t="inlineStr"/>
@@ -25616,18 +25384,10 @@
       <c r="CJ168" t="inlineStr"/>
       <c r="CK168" t="inlineStr"/>
       <c r="CL168" t="inlineStr"/>
-      <c r="CM168" t="n">
-        <v>220.76</v>
-      </c>
-      <c r="CN168" t="n">
-        <v>214.99</v>
-      </c>
-      <c r="CO168" t="n">
-        <v>194.93</v>
-      </c>
-      <c r="CP168" t="n">
-        <v>171.74</v>
-      </c>
+      <c r="CM168" t="inlineStr"/>
+      <c r="CN168" t="inlineStr"/>
+      <c r="CO168" t="inlineStr"/>
+      <c r="CP168" t="inlineStr"/>
     </row>
     <row r="169">
       <c r="A169" t="n">
@@ -27035,24 +26795,12 @@
       <c r="BK177" t="inlineStr"/>
       <c r="BL177" t="inlineStr"/>
       <c r="BM177" t="inlineStr"/>
-      <c r="BN177" t="n">
-        <v>0</v>
-      </c>
-      <c r="BO177" t="n">
-        <v>1139.91</v>
-      </c>
-      <c r="BP177" t="n">
-        <v>1181.23</v>
-      </c>
-      <c r="BQ177" t="n">
-        <v>1169.45</v>
-      </c>
-      <c r="BR177" t="n">
-        <v>122.18</v>
-      </c>
-      <c r="BS177" t="n">
-        <v>219</v>
-      </c>
+      <c r="BN177" t="inlineStr"/>
+      <c r="BO177" t="inlineStr"/>
+      <c r="BP177" t="inlineStr"/>
+      <c r="BQ177" t="inlineStr"/>
+      <c r="BR177" t="inlineStr"/>
+      <c r="BS177" t="inlineStr"/>
       <c r="BT177" t="inlineStr"/>
       <c r="BU177" t="inlineStr"/>
       <c r="BV177" t="inlineStr"/>
@@ -27072,18 +26820,10 @@
       <c r="CJ177" t="inlineStr"/>
       <c r="CK177" t="inlineStr"/>
       <c r="CL177" t="inlineStr"/>
-      <c r="CM177" t="n">
-        <v>6568.45</v>
-      </c>
-      <c r="CN177" t="n">
-        <v>506.9</v>
-      </c>
-      <c r="CO177" t="n">
-        <v>464.68</v>
-      </c>
-      <c r="CP177" t="n">
-        <v>641</v>
-      </c>
+      <c r="CM177" t="inlineStr"/>
+      <c r="CN177" t="inlineStr"/>
+      <c r="CO177" t="inlineStr"/>
+      <c r="CP177" t="inlineStr"/>
     </row>
     <row r="178">
       <c r="A178" t="n">
@@ -29367,18 +29107,10 @@
       <c r="BA192" t="n">
         <v>2007</v>
       </c>
-      <c r="BB192" t="n">
-        <v>153.28</v>
-      </c>
-      <c r="BC192" t="n">
-        <v>156.48</v>
-      </c>
-      <c r="BD192" t="n">
-        <v>91.44</v>
-      </c>
-      <c r="BE192" t="n">
-        <v>95.17</v>
-      </c>
+      <c r="BB192" t="inlineStr"/>
+      <c r="BC192" t="inlineStr"/>
+      <c r="BD192" t="inlineStr"/>
+      <c r="BE192" t="inlineStr"/>
       <c r="BF192" t="inlineStr"/>
       <c r="BG192" t="inlineStr"/>
       <c r="BH192" t="inlineStr"/>
@@ -29412,18 +29144,10 @@
       <c r="CJ192" t="inlineStr"/>
       <c r="CK192" t="inlineStr"/>
       <c r="CL192" t="inlineStr"/>
-      <c r="CM192" t="n">
-        <v>95.17</v>
-      </c>
-      <c r="CN192" t="n">
-        <v>112.94</v>
-      </c>
-      <c r="CO192" t="n">
-        <v>123.52</v>
-      </c>
-      <c r="CP192" t="n">
-        <v>108.78</v>
-      </c>
+      <c r="CM192" t="inlineStr"/>
+      <c r="CN192" t="inlineStr"/>
+      <c r="CO192" t="inlineStr"/>
+      <c r="CP192" t="inlineStr"/>
     </row>
     <row r="193">
       <c r="A193" t="n">
@@ -29525,18 +29249,10 @@
       <c r="BA193" t="n">
         <v>2007</v>
       </c>
-      <c r="BB193" t="n">
-        <v>17.98</v>
-      </c>
-      <c r="BC193" t="n">
-        <v>17.98</v>
-      </c>
-      <c r="BD193" t="n">
-        <v>17.98</v>
-      </c>
-      <c r="BE193" t="n">
-        <v>17.98</v>
-      </c>
+      <c r="BB193" t="inlineStr"/>
+      <c r="BC193" t="inlineStr"/>
+      <c r="BD193" t="inlineStr"/>
+      <c r="BE193" t="inlineStr"/>
       <c r="BF193" t="inlineStr"/>
       <c r="BG193" t="inlineStr"/>
       <c r="BH193" t="inlineStr"/>
@@ -29570,18 +29286,10 @@
       <c r="CJ193" t="inlineStr"/>
       <c r="CK193" t="inlineStr"/>
       <c r="CL193" t="inlineStr"/>
-      <c r="CM193" t="n">
-        <v>17.98</v>
-      </c>
-      <c r="CN193" t="n">
-        <v>9248.67</v>
-      </c>
-      <c r="CO193" t="n">
-        <v>9267.91</v>
-      </c>
-      <c r="CP193" t="n">
-        <v>9267.91</v>
-      </c>
+      <c r="CM193" t="inlineStr"/>
+      <c r="CN193" t="inlineStr"/>
+      <c r="CO193" t="inlineStr"/>
+      <c r="CP193" t="inlineStr"/>
     </row>
     <row r="194">
       <c r="A194" t="n">
@@ -30289,18 +29997,10 @@
       <c r="BC198" t="inlineStr"/>
       <c r="BD198" t="inlineStr"/>
       <c r="BE198" t="inlineStr"/>
-      <c r="BF198" t="n">
-        <v>62.53</v>
-      </c>
-      <c r="BG198" t="n">
-        <v>57.25</v>
-      </c>
-      <c r="BH198" t="n">
-        <v>126.46</v>
-      </c>
-      <c r="BI198" t="n">
-        <v>280.45</v>
-      </c>
+      <c r="BF198" t="inlineStr"/>
+      <c r="BG198" t="inlineStr"/>
+      <c r="BH198" t="inlineStr"/>
+      <c r="BI198" t="inlineStr"/>
       <c r="BJ198" t="inlineStr"/>
       <c r="BK198" t="inlineStr"/>
       <c r="BL198" t="inlineStr"/>
@@ -30330,18 +30030,10 @@
       <c r="CJ198" t="inlineStr"/>
       <c r="CK198" t="inlineStr"/>
       <c r="CL198" t="inlineStr"/>
-      <c r="CM198" t="n">
-        <v>165.24</v>
-      </c>
-      <c r="CN198" t="n">
-        <v>150.74</v>
-      </c>
-      <c r="CO198" t="n">
-        <v>162.87</v>
-      </c>
-      <c r="CP198" t="n">
-        <v>152.63</v>
-      </c>
+      <c r="CM198" t="inlineStr"/>
+      <c r="CN198" t="inlineStr"/>
+      <c r="CO198" t="inlineStr"/>
+      <c r="CP198" t="inlineStr"/>
     </row>
     <row r="199">
       <c r="A199" t="n">
@@ -30464,18 +30156,10 @@
       <c r="BF199" t="inlineStr"/>
       <c r="BG199" t="inlineStr"/>
       <c r="BH199" t="inlineStr"/>
-      <c r="BI199" t="n">
-        <v>663.85</v>
-      </c>
-      <c r="BJ199" t="n">
-        <v>341.79</v>
-      </c>
-      <c r="BK199" t="n">
-        <v>341.94</v>
-      </c>
-      <c r="BL199" t="n">
-        <v>342.01</v>
-      </c>
+      <c r="BI199" t="inlineStr"/>
+      <c r="BJ199" t="inlineStr"/>
+      <c r="BK199" t="inlineStr"/>
+      <c r="BL199" t="inlineStr"/>
       <c r="BM199" t="inlineStr"/>
       <c r="BN199" t="inlineStr"/>
       <c r="BO199" t="inlineStr"/>
@@ -30502,18 +30186,10 @@
       <c r="CJ199" t="inlineStr"/>
       <c r="CK199" t="inlineStr"/>
       <c r="CL199" t="inlineStr"/>
-      <c r="CM199" t="n">
-        <v>1056.26</v>
-      </c>
-      <c r="CN199" t="n">
-        <v>1056.47</v>
-      </c>
-      <c r="CO199" t="n">
-        <v>1251.03</v>
-      </c>
-      <c r="CP199" t="n">
-        <v>109.76</v>
-      </c>
+      <c r="CM199" t="inlineStr"/>
+      <c r="CN199" t="inlineStr"/>
+      <c r="CO199" t="inlineStr"/>
+      <c r="CP199" t="inlineStr"/>
     </row>
     <row r="200">
       <c r="A200" t="n">
@@ -30905,18 +30581,10 @@
       <c r="BA202" t="n">
         <v>2005</v>
       </c>
-      <c r="BB202" t="n">
-        <v>183.44</v>
-      </c>
-      <c r="BC202" t="n">
-        <v>173.5</v>
-      </c>
-      <c r="BD202" t="n">
-        <v>185.62</v>
-      </c>
-      <c r="BE202" t="n">
-        <v>177.9</v>
-      </c>
+      <c r="BB202" t="inlineStr"/>
+      <c r="BC202" t="inlineStr"/>
+      <c r="BD202" t="inlineStr"/>
+      <c r="BE202" t="inlineStr"/>
       <c r="BF202" t="inlineStr"/>
       <c r="BG202" t="inlineStr"/>
       <c r="BH202" t="inlineStr"/>
@@ -30950,18 +30618,10 @@
       <c r="CJ202" t="inlineStr"/>
       <c r="CK202" t="inlineStr"/>
       <c r="CL202" t="inlineStr"/>
-      <c r="CM202" t="n">
-        <v>145.53</v>
-      </c>
-      <c r="CN202" t="n">
-        <v>99.56999999999999</v>
-      </c>
-      <c r="CO202" t="n">
-        <v>92.84</v>
-      </c>
-      <c r="CP202" t="n">
-        <v>219.63</v>
-      </c>
+      <c r="CM202" t="inlineStr"/>
+      <c r="CN202" t="inlineStr"/>
+      <c r="CO202" t="inlineStr"/>
+      <c r="CP202" t="inlineStr"/>
     </row>
     <row r="203">
       <c r="A203" t="n">
@@ -31356,12 +31016,8 @@
       <c r="BB205" t="inlineStr"/>
       <c r="BC205" t="inlineStr"/>
       <c r="BD205" t="inlineStr"/>
-      <c r="BE205" t="n">
-        <v>320.45</v>
-      </c>
-      <c r="BF205" t="n">
-        <v>285.8</v>
-      </c>
+      <c r="BE205" t="inlineStr"/>
+      <c r="BF205" t="inlineStr"/>
       <c r="BG205" t="inlineStr"/>
       <c r="BH205" t="inlineStr"/>
       <c r="BI205" t="inlineStr"/>
@@ -31394,18 +31050,10 @@
       <c r="CJ205" t="inlineStr"/>
       <c r="CK205" t="inlineStr"/>
       <c r="CL205" t="inlineStr"/>
-      <c r="CM205" t="n">
-        <v>114.08</v>
-      </c>
-      <c r="CN205" t="n">
-        <v>163.49</v>
-      </c>
-      <c r="CO205" t="n">
-        <v>143.32</v>
-      </c>
-      <c r="CP205" t="n">
-        <v>2216.12</v>
-      </c>
+      <c r="CM205" t="inlineStr"/>
+      <c r="CN205" t="inlineStr"/>
+      <c r="CO205" t="inlineStr"/>
+      <c r="CP205" t="inlineStr"/>
     </row>
     <row r="206">
       <c r="A206" t="n">
@@ -31983,24 +31631,12 @@
       <c r="BA209" t="n">
         <v>2006</v>
       </c>
-      <c r="BB209" t="n">
-        <v>28.41</v>
-      </c>
-      <c r="BC209" t="n">
-        <v>32.59</v>
-      </c>
-      <c r="BD209" t="n">
-        <v>46.65</v>
-      </c>
-      <c r="BE209" t="n">
-        <v>46.57</v>
-      </c>
-      <c r="BF209" t="n">
-        <v>42.63</v>
-      </c>
-      <c r="BG209" t="n">
-        <v>43.38</v>
-      </c>
+      <c r="BB209" t="inlineStr"/>
+      <c r="BC209" t="inlineStr"/>
+      <c r="BD209" t="inlineStr"/>
+      <c r="BE209" t="inlineStr"/>
+      <c r="BF209" t="inlineStr"/>
+      <c r="BG209" t="inlineStr"/>
       <c r="BH209" t="inlineStr"/>
       <c r="BI209" t="inlineStr"/>
       <c r="BJ209" t="inlineStr"/>
@@ -32032,18 +31668,10 @@
       <c r="CJ209" t="inlineStr"/>
       <c r="CK209" t="inlineStr"/>
       <c r="CL209" t="inlineStr"/>
-      <c r="CM209" t="n">
-        <v>48.17</v>
-      </c>
-      <c r="CN209" t="n">
-        <v>50.56</v>
-      </c>
-      <c r="CO209" t="n">
-        <v>48.31</v>
-      </c>
-      <c r="CP209" t="n">
-        <v>48.87</v>
-      </c>
+      <c r="CM209" t="inlineStr"/>
+      <c r="CN209" t="inlineStr"/>
+      <c r="CO209" t="inlineStr"/>
+      <c r="CP209" t="inlineStr"/>
     </row>
     <row r="210">
       <c r="A210" t="n">
@@ -32157,27 +31785,13 @@
       </c>
       <c r="BB210" t="inlineStr"/>
       <c r="BC210" t="inlineStr"/>
-      <c r="BD210" t="n">
-        <v>663.85</v>
-      </c>
-      <c r="BE210" t="n">
-        <v>341.79</v>
-      </c>
-      <c r="BF210" t="n">
-        <v>341.94</v>
-      </c>
-      <c r="BG210" t="n">
-        <v>342.01</v>
-      </c>
-      <c r="BH210" t="n">
-        <v>1056.26</v>
-      </c>
-      <c r="BI210" t="n">
-        <v>1056.47</v>
-      </c>
-      <c r="BJ210" t="n">
-        <v>1251.03</v>
-      </c>
+      <c r="BD210" t="inlineStr"/>
+      <c r="BE210" t="inlineStr"/>
+      <c r="BF210" t="inlineStr"/>
+      <c r="BG210" t="inlineStr"/>
+      <c r="BH210" t="inlineStr"/>
+      <c r="BI210" t="inlineStr"/>
+      <c r="BJ210" t="inlineStr"/>
       <c r="BK210" t="inlineStr"/>
       <c r="BL210" t="inlineStr"/>
       <c r="BM210" t="inlineStr"/>
@@ -32206,18 +31820,10 @@
       <c r="CJ210" t="inlineStr"/>
       <c r="CK210" t="inlineStr"/>
       <c r="CL210" t="inlineStr"/>
-      <c r="CM210" t="n">
-        <v>109.76</v>
-      </c>
-      <c r="CN210" t="n">
-        <v>1294.8</v>
-      </c>
-      <c r="CO210" t="n">
-        <v>124.96</v>
-      </c>
-      <c r="CP210" t="n">
-        <v>950.66</v>
-      </c>
+      <c r="CM210" t="inlineStr"/>
+      <c r="CN210" t="inlineStr"/>
+      <c r="CO210" t="inlineStr"/>
+      <c r="CP210" t="inlineStr"/>
     </row>
     <row r="211">
       <c r="A211" t="n">
@@ -32656,27 +32262,13 @@
       <c r="BF213" t="inlineStr"/>
       <c r="BG213" t="inlineStr"/>
       <c r="BH213" t="inlineStr"/>
-      <c r="BI213" t="n">
-        <v>444.25</v>
-      </c>
-      <c r="BJ213" t="n">
-        <v>459.86</v>
-      </c>
-      <c r="BK213" t="n">
-        <v>41.13</v>
-      </c>
-      <c r="BL213" t="n">
-        <v>33.33</v>
-      </c>
-      <c r="BM213" t="n">
-        <v>29.01</v>
-      </c>
-      <c r="BN213" t="n">
-        <v>126.98</v>
-      </c>
-      <c r="BO213" t="n">
-        <v>44.95</v>
-      </c>
+      <c r="BI213" t="inlineStr"/>
+      <c r="BJ213" t="inlineStr"/>
+      <c r="BK213" t="inlineStr"/>
+      <c r="BL213" t="inlineStr"/>
+      <c r="BM213" t="inlineStr"/>
+      <c r="BN213" t="inlineStr"/>
+      <c r="BO213" t="inlineStr"/>
       <c r="BP213" t="inlineStr"/>
       <c r="BQ213" t="inlineStr"/>
       <c r="BR213" t="inlineStr"/>
@@ -32700,18 +32292,10 @@
       <c r="CJ213" t="inlineStr"/>
       <c r="CK213" t="inlineStr"/>
       <c r="CL213" t="inlineStr"/>
-      <c r="CM213" t="n">
-        <v>54.16</v>
-      </c>
-      <c r="CN213" t="n">
-        <v>61.72</v>
-      </c>
-      <c r="CO213" t="n">
-        <v>22.18</v>
-      </c>
-      <c r="CP213" t="n">
-        <v>51.43</v>
-      </c>
+      <c r="CM213" t="inlineStr"/>
+      <c r="CN213" t="inlineStr"/>
+      <c r="CO213" t="inlineStr"/>
+      <c r="CP213" t="inlineStr"/>
     </row>
     <row r="214">
       <c r="A214" t="n">
@@ -32815,21 +32399,11 @@
       <c r="BA214" t="n">
         <v>2005</v>
       </c>
-      <c r="BB214" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC214" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD214" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE214" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF214" t="n">
-        <v>0</v>
-      </c>
+      <c r="BB214" t="inlineStr"/>
+      <c r="BC214" t="inlineStr"/>
+      <c r="BD214" t="inlineStr"/>
+      <c r="BE214" t="inlineStr"/>
+      <c r="BF214" t="inlineStr"/>
       <c r="BG214" t="inlineStr"/>
       <c r="BH214" t="inlineStr"/>
       <c r="BI214" t="inlineStr"/>
@@ -32862,18 +32436,10 @@
       <c r="CJ214" t="inlineStr"/>
       <c r="CK214" t="inlineStr"/>
       <c r="CL214" t="inlineStr"/>
-      <c r="CM214" t="n">
-        <v>224.46</v>
-      </c>
-      <c r="CN214" t="n">
-        <v>360.32</v>
-      </c>
-      <c r="CO214" t="n">
-        <v>340.1</v>
-      </c>
-      <c r="CP214" t="n">
-        <v>437.09</v>
-      </c>
+      <c r="CM214" t="inlineStr"/>
+      <c r="CN214" t="inlineStr"/>
+      <c r="CO214" t="inlineStr"/>
+      <c r="CP214" t="inlineStr"/>
     </row>
     <row r="215">
       <c r="A215" t="n">
@@ -33117,21 +32683,11 @@
       <c r="BA216" t="n">
         <v>2005</v>
       </c>
-      <c r="BB216" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC216" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD216" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="BE216" t="n">
-        <v>1449.03</v>
-      </c>
-      <c r="BF216" t="n">
-        <v>1645.82</v>
-      </c>
+      <c r="BB216" t="inlineStr"/>
+      <c r="BC216" t="inlineStr"/>
+      <c r="BD216" t="inlineStr"/>
+      <c r="BE216" t="inlineStr"/>
+      <c r="BF216" t="inlineStr"/>
       <c r="BG216" t="inlineStr"/>
       <c r="BH216" t="inlineStr"/>
       <c r="BI216" t="inlineStr"/>
@@ -33164,18 +32720,10 @@
       <c r="CJ216" t="inlineStr"/>
       <c r="CK216" t="inlineStr"/>
       <c r="CL216" t="inlineStr"/>
-      <c r="CM216" t="n">
-        <v>1657.11</v>
-      </c>
-      <c r="CN216" t="n">
-        <v>2112.05</v>
-      </c>
-      <c r="CO216" t="n">
-        <v>2114.11</v>
-      </c>
-      <c r="CP216" t="n">
-        <v>2803.51</v>
-      </c>
+      <c r="CM216" t="inlineStr"/>
+      <c r="CN216" t="inlineStr"/>
+      <c r="CO216" t="inlineStr"/>
+      <c r="CP216" t="inlineStr"/>
     </row>
     <row r="217">
       <c r="A217" t="n">
@@ -33429,21 +32977,11 @@
       </c>
       <c r="BB218" t="inlineStr"/>
       <c r="BC218" t="inlineStr"/>
-      <c r="BD218" t="n">
-        <v>198.69</v>
-      </c>
-      <c r="BE218" t="n">
-        <v>192.92</v>
-      </c>
-      <c r="BF218" t="n">
-        <v>162.45</v>
-      </c>
-      <c r="BG218" t="n">
-        <v>156.54</v>
-      </c>
-      <c r="BH218" t="n">
-        <v>153.28</v>
-      </c>
+      <c r="BD218" t="inlineStr"/>
+      <c r="BE218" t="inlineStr"/>
+      <c r="BF218" t="inlineStr"/>
+      <c r="BG218" t="inlineStr"/>
+      <c r="BH218" t="inlineStr"/>
       <c r="BI218" t="inlineStr"/>
       <c r="BJ218" t="inlineStr"/>
       <c r="BK218" t="inlineStr"/>
@@ -33474,18 +33012,10 @@
       <c r="CJ218" t="inlineStr"/>
       <c r="CK218" t="inlineStr"/>
       <c r="CL218" t="inlineStr"/>
-      <c r="CM218" t="n">
-        <v>156.48</v>
-      </c>
-      <c r="CN218" t="n">
-        <v>91.44</v>
-      </c>
-      <c r="CO218" t="n">
-        <v>95.17</v>
-      </c>
-      <c r="CP218" t="n">
-        <v>112.94</v>
-      </c>
+      <c r="CM218" t="inlineStr"/>
+      <c r="CN218" t="inlineStr"/>
+      <c r="CO218" t="inlineStr"/>
+      <c r="CP218" t="inlineStr"/>
     </row>
     <row r="219">
       <c r="A219" t="n">
@@ -33595,21 +33125,11 @@
       </c>
       <c r="BB219" t="inlineStr"/>
       <c r="BC219" t="inlineStr"/>
-      <c r="BD219" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE219" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF219" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG219" t="n">
-        <v>18.4</v>
-      </c>
-      <c r="BH219" t="n">
-        <v>17.98</v>
-      </c>
+      <c r="BD219" t="inlineStr"/>
+      <c r="BE219" t="inlineStr"/>
+      <c r="BF219" t="inlineStr"/>
+      <c r="BG219" t="inlineStr"/>
+      <c r="BH219" t="inlineStr"/>
       <c r="BI219" t="inlineStr"/>
       <c r="BJ219" t="inlineStr"/>
       <c r="BK219" t="inlineStr"/>
@@ -33640,18 +33160,10 @@
       <c r="CJ219" t="inlineStr"/>
       <c r="CK219" t="inlineStr"/>
       <c r="CL219" t="inlineStr"/>
-      <c r="CM219" t="n">
-        <v>17.98</v>
-      </c>
-      <c r="CN219" t="n">
-        <v>17.98</v>
-      </c>
-      <c r="CO219" t="n">
-        <v>17.98</v>
-      </c>
-      <c r="CP219" t="n">
-        <v>9248.67</v>
-      </c>
+      <c r="CM219" t="inlineStr"/>
+      <c r="CN219" t="inlineStr"/>
+      <c r="CO219" t="inlineStr"/>
+      <c r="CP219" t="inlineStr"/>
     </row>
     <row r="220">
       <c r="A220" t="n">
@@ -33893,21 +33405,11 @@
       <c r="BA221" t="n">
         <v>2009</v>
       </c>
-      <c r="BB221" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC221" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD221" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE221" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF221" t="n">
-        <v>0</v>
-      </c>
+      <c r="BB221" t="inlineStr"/>
+      <c r="BC221" t="inlineStr"/>
+      <c r="BD221" t="inlineStr"/>
+      <c r="BE221" t="inlineStr"/>
+      <c r="BF221" t="inlineStr"/>
       <c r="BG221" t="inlineStr"/>
       <c r="BH221" t="inlineStr"/>
       <c r="BI221" t="inlineStr"/>
@@ -33940,18 +33442,10 @@
       <c r="CJ221" t="inlineStr"/>
       <c r="CK221" t="inlineStr"/>
       <c r="CL221" t="inlineStr"/>
-      <c r="CM221" t="n">
-        <v>3800.33</v>
-      </c>
-      <c r="CN221" t="n">
-        <v>155.62</v>
-      </c>
-      <c r="CO221" t="n">
-        <v>138.06</v>
-      </c>
-      <c r="CP221" t="n">
-        <v>149.69</v>
-      </c>
+      <c r="CM221" t="inlineStr"/>
+      <c r="CN221" t="inlineStr"/>
+      <c r="CO221" t="inlineStr"/>
+      <c r="CP221" t="inlineStr"/>
     </row>
     <row r="222">
       <c r="A222" t="n">
@@ -34058,21 +33552,11 @@
         <v>2005</v>
       </c>
       <c r="BB222" t="inlineStr"/>
-      <c r="BC222" t="n">
-        <v>11.81</v>
-      </c>
-      <c r="BD222" t="n">
-        <v>12.51</v>
-      </c>
-      <c r="BE222" t="n">
-        <v>16.73</v>
-      </c>
-      <c r="BF222" t="n">
-        <v>57.95</v>
-      </c>
-      <c r="BG222" t="n">
-        <v>59.06</v>
-      </c>
+      <c r="BC222" t="inlineStr"/>
+      <c r="BD222" t="inlineStr"/>
+      <c r="BE222" t="inlineStr"/>
+      <c r="BF222" t="inlineStr"/>
+      <c r="BG222" t="inlineStr"/>
       <c r="BH222" t="inlineStr"/>
       <c r="BI222" t="inlineStr"/>
       <c r="BJ222" t="inlineStr"/>
@@ -34104,18 +33588,10 @@
       <c r="CJ222" t="inlineStr"/>
       <c r="CK222" t="inlineStr"/>
       <c r="CL222" t="inlineStr"/>
-      <c r="CM222" t="n">
-        <v>53.63</v>
-      </c>
-      <c r="CN222" t="n">
-        <v>52.33</v>
-      </c>
-      <c r="CO222" t="n">
-        <v>51.75</v>
-      </c>
-      <c r="CP222" t="n">
-        <v>55.37</v>
-      </c>
+      <c r="CM222" t="inlineStr"/>
+      <c r="CN222" t="inlineStr"/>
+      <c r="CO222" t="inlineStr"/>
+      <c r="CP222" t="inlineStr"/>
     </row>
     <row r="223">
       <c r="A223" t="n">
@@ -34222,21 +33698,11 @@
         <v>2005</v>
       </c>
       <c r="BB223" t="inlineStr"/>
-      <c r="BC223" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD223" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE223" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF223" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="BG223" t="n">
-        <v>9.630000000000001</v>
-      </c>
+      <c r="BC223" t="inlineStr"/>
+      <c r="BD223" t="inlineStr"/>
+      <c r="BE223" t="inlineStr"/>
+      <c r="BF223" t="inlineStr"/>
+      <c r="BG223" t="inlineStr"/>
       <c r="BH223" t="inlineStr"/>
       <c r="BI223" t="inlineStr"/>
       <c r="BJ223" t="inlineStr"/>
@@ -34268,18 +33734,10 @@
       <c r="CJ223" t="inlineStr"/>
       <c r="CK223" t="inlineStr"/>
       <c r="CL223" t="inlineStr"/>
-      <c r="CM223" t="n">
-        <v>29.48</v>
-      </c>
-      <c r="CN223" t="n">
-        <v>12.95</v>
-      </c>
-      <c r="CO223" t="n">
-        <v>10.82</v>
-      </c>
-      <c r="CP223" t="n">
-        <v>21.26</v>
-      </c>
+      <c r="CM223" t="inlineStr"/>
+      <c r="CN223" t="inlineStr"/>
+      <c r="CO223" t="inlineStr"/>
+      <c r="CP223" t="inlineStr"/>
     </row>
     <row r="224">
       <c r="A224" t="n">
@@ -34528,21 +33986,11 @@
         <v>2005</v>
       </c>
       <c r="BB225" t="inlineStr"/>
-      <c r="BC225" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD225" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE225" t="n">
-        <v>4420.92</v>
-      </c>
-      <c r="BF225" t="n">
-        <v>4420.92</v>
-      </c>
-      <c r="BG225" t="n">
-        <v>0</v>
-      </c>
+      <c r="BC225" t="inlineStr"/>
+      <c r="BD225" t="inlineStr"/>
+      <c r="BE225" t="inlineStr"/>
+      <c r="BF225" t="inlineStr"/>
+      <c r="BG225" t="inlineStr"/>
       <c r="BH225" t="inlineStr"/>
       <c r="BI225" t="inlineStr"/>
       <c r="BJ225" t="inlineStr"/>
@@ -34574,18 +34022,10 @@
       <c r="CJ225" t="inlineStr"/>
       <c r="CK225" t="inlineStr"/>
       <c r="CL225" t="inlineStr"/>
-      <c r="CM225" t="n">
-        <v>0</v>
-      </c>
-      <c r="CN225" t="n">
-        <v>0</v>
-      </c>
-      <c r="CO225" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP225" t="n">
-        <v>0</v>
-      </c>
+      <c r="CM225" t="inlineStr"/>
+      <c r="CN225" t="inlineStr"/>
+      <c r="CO225" t="inlineStr"/>
+      <c r="CP225" t="inlineStr"/>
     </row>
     <row r="226">
       <c r="A226" t="n">
@@ -34692,21 +34132,11 @@
         <v>2005</v>
       </c>
       <c r="BB226" t="inlineStr"/>
-      <c r="BC226" t="n">
-        <v>199.39</v>
-      </c>
-      <c r="BD226" t="n">
-        <v>208.36</v>
-      </c>
-      <c r="BE226" t="n">
-        <v>214.86</v>
-      </c>
-      <c r="BF226" t="n">
-        <v>223.98</v>
-      </c>
-      <c r="BG226" t="n">
-        <v>221.12</v>
-      </c>
+      <c r="BC226" t="inlineStr"/>
+      <c r="BD226" t="inlineStr"/>
+      <c r="BE226" t="inlineStr"/>
+      <c r="BF226" t="inlineStr"/>
+      <c r="BG226" t="inlineStr"/>
       <c r="BH226" t="inlineStr"/>
       <c r="BI226" t="inlineStr"/>
       <c r="BJ226" t="inlineStr"/>
@@ -34738,18 +34168,10 @@
       <c r="CJ226" t="inlineStr"/>
       <c r="CK226" t="inlineStr"/>
       <c r="CL226" t="inlineStr"/>
-      <c r="CM226" t="n">
-        <v>187.21</v>
-      </c>
-      <c r="CN226" t="n">
-        <v>140.06</v>
-      </c>
-      <c r="CO226" t="n">
-        <v>130.46</v>
-      </c>
-      <c r="CP226" t="n">
-        <v>169.96</v>
-      </c>
+      <c r="CM226" t="inlineStr"/>
+      <c r="CN226" t="inlineStr"/>
+      <c r="CO226" t="inlineStr"/>
+      <c r="CP226" t="inlineStr"/>
     </row>
     <row r="227">
       <c r="A227" t="n">
@@ -34998,21 +34420,11 @@
         <v>2005</v>
       </c>
       <c r="BB228" t="inlineStr"/>
-      <c r="BC228" t="n">
-        <v>70.97</v>
-      </c>
-      <c r="BD228" t="n">
-        <v>67.62</v>
-      </c>
-      <c r="BE228" t="n">
-        <v>63.14</v>
-      </c>
-      <c r="BF228" t="n">
-        <v>61.27</v>
-      </c>
-      <c r="BG228" t="n">
-        <v>36.2</v>
-      </c>
+      <c r="BC228" t="inlineStr"/>
+      <c r="BD228" t="inlineStr"/>
+      <c r="BE228" t="inlineStr"/>
+      <c r="BF228" t="inlineStr"/>
+      <c r="BG228" t="inlineStr"/>
       <c r="BH228" t="inlineStr"/>
       <c r="BI228" t="inlineStr"/>
       <c r="BJ228" t="inlineStr"/>
@@ -35044,18 +34456,10 @@
       <c r="CJ228" t="inlineStr"/>
       <c r="CK228" t="inlineStr"/>
       <c r="CL228" t="inlineStr"/>
-      <c r="CM228" t="n">
-        <v>51.56</v>
-      </c>
-      <c r="CN228" t="n">
-        <v>38.99</v>
-      </c>
-      <c r="CO228" t="n">
-        <v>36.92</v>
-      </c>
-      <c r="CP228" t="n">
-        <v>42.73</v>
-      </c>
+      <c r="CM228" t="inlineStr"/>
+      <c r="CN228" t="inlineStr"/>
+      <c r="CO228" t="inlineStr"/>
+      <c r="CP228" t="inlineStr"/>
     </row>
     <row r="229">
       <c r="A229" t="n">
@@ -35627,15 +35031,9 @@
       </c>
       <c r="BB232" t="inlineStr"/>
       <c r="BC232" t="inlineStr"/>
-      <c r="BD232" t="n">
-        <v>297.04</v>
-      </c>
-      <c r="BE232" t="n">
-        <v>183.59</v>
-      </c>
-      <c r="BF232" t="n">
-        <v>263.55</v>
-      </c>
+      <c r="BD232" t="inlineStr"/>
+      <c r="BE232" t="inlineStr"/>
+      <c r="BF232" t="inlineStr"/>
       <c r="BG232" t="inlineStr"/>
       <c r="BH232" t="inlineStr"/>
       <c r="BI232" t="inlineStr"/>
@@ -35668,18 +35066,10 @@
       <c r="CJ232" t="inlineStr"/>
       <c r="CK232" t="inlineStr"/>
       <c r="CL232" t="inlineStr"/>
-      <c r="CM232" t="n">
-        <v>324.2</v>
-      </c>
-      <c r="CN232" t="n">
-        <v>280.32</v>
-      </c>
-      <c r="CO232" t="n">
-        <v>327.77</v>
-      </c>
-      <c r="CP232" t="n">
-        <v>363.14</v>
-      </c>
+      <c r="CM232" t="inlineStr"/>
+      <c r="CN232" t="inlineStr"/>
+      <c r="CO232" t="inlineStr"/>
+      <c r="CP232" t="inlineStr"/>
     </row>
     <row r="233">
       <c r="A233" t="n">
@@ -35784,18 +35174,10 @@
         <v>2004</v>
       </c>
       <c r="BB233" t="inlineStr"/>
-      <c r="BC233" t="n">
-        <v>313.24</v>
-      </c>
-      <c r="BD233" t="n">
-        <v>283.67</v>
-      </c>
-      <c r="BE233" t="n">
-        <v>170.89</v>
-      </c>
-      <c r="BF233" t="n">
-        <v>276.8</v>
-      </c>
+      <c r="BC233" t="inlineStr"/>
+      <c r="BD233" t="inlineStr"/>
+      <c r="BE233" t="inlineStr"/>
+      <c r="BF233" t="inlineStr"/>
       <c r="BG233" t="inlineStr"/>
       <c r="BH233" t="inlineStr"/>
       <c r="BI233" t="inlineStr"/>
@@ -35828,18 +35210,10 @@
       <c r="CJ233" t="inlineStr"/>
       <c r="CK233" t="inlineStr"/>
       <c r="CL233" t="inlineStr"/>
-      <c r="CM233" t="n">
-        <v>410.98</v>
-      </c>
-      <c r="CN233" t="n">
-        <v>423.28</v>
-      </c>
-      <c r="CO233" t="n">
-        <v>461.5</v>
-      </c>
-      <c r="CP233" t="n">
-        <v>463.58</v>
-      </c>
+      <c r="CM233" t="inlineStr"/>
+      <c r="CN233" t="inlineStr"/>
+      <c r="CO233" t="inlineStr"/>
+      <c r="CP233" t="inlineStr"/>
     </row>
     <row r="234">
       <c r="A234" t="n">
@@ -35944,18 +35318,10 @@
         <v>2004</v>
       </c>
       <c r="BB234" t="inlineStr"/>
-      <c r="BC234" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD234" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE234" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF234" t="n">
-        <v>5061.24</v>
-      </c>
+      <c r="BC234" t="inlineStr"/>
+      <c r="BD234" t="inlineStr"/>
+      <c r="BE234" t="inlineStr"/>
+      <c r="BF234" t="inlineStr"/>
       <c r="BG234" t="inlineStr"/>
       <c r="BH234" t="inlineStr"/>
       <c r="BI234" t="inlineStr"/>
@@ -35988,18 +35354,10 @@
       <c r="CJ234" t="inlineStr"/>
       <c r="CK234" t="inlineStr"/>
       <c r="CL234" t="inlineStr"/>
-      <c r="CM234" t="n">
-        <v>4124.97</v>
-      </c>
-      <c r="CN234" t="n">
-        <v>1294.96</v>
-      </c>
-      <c r="CO234" t="n">
-        <v>1219.01</v>
-      </c>
-      <c r="CP234" t="n">
-        <v>427.24</v>
-      </c>
+      <c r="CM234" t="inlineStr"/>
+      <c r="CN234" t="inlineStr"/>
+      <c r="CO234" t="inlineStr"/>
+      <c r="CP234" t="inlineStr"/>
     </row>
     <row r="235">
       <c r="A235" t="n">
@@ -36104,18 +35462,10 @@
         <v>2004</v>
       </c>
       <c r="BB235" t="inlineStr"/>
-      <c r="BC235" t="n">
-        <v>214.06</v>
-      </c>
-      <c r="BD235" t="n">
-        <v>151.52</v>
-      </c>
-      <c r="BE235" t="n">
-        <v>5016.63</v>
-      </c>
-      <c r="BF235" t="n">
-        <v>108.53</v>
-      </c>
+      <c r="BC235" t="inlineStr"/>
+      <c r="BD235" t="inlineStr"/>
+      <c r="BE235" t="inlineStr"/>
+      <c r="BF235" t="inlineStr"/>
       <c r="BG235" t="inlineStr"/>
       <c r="BH235" t="inlineStr"/>
       <c r="BI235" t="inlineStr"/>
@@ -36148,18 +35498,10 @@
       <c r="CJ235" t="inlineStr"/>
       <c r="CK235" t="inlineStr"/>
       <c r="CL235" t="inlineStr"/>
-      <c r="CM235" t="n">
-        <v>148.96</v>
-      </c>
-      <c r="CN235" t="n">
-        <v>83.06</v>
-      </c>
-      <c r="CO235" t="n">
-        <v>81.22</v>
-      </c>
-      <c r="CP235" t="n">
-        <v>85.47</v>
-      </c>
+      <c r="CM235" t="inlineStr"/>
+      <c r="CN235" t="inlineStr"/>
+      <c r="CO235" t="inlineStr"/>
+      <c r="CP235" t="inlineStr"/>
     </row>
     <row r="236">
       <c r="A236" t="n">
@@ -36261,18 +35603,10 @@
       <c r="BA236" t="n">
         <v>2004</v>
       </c>
-      <c r="BB236" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC236" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD236" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE236" t="n">
-        <v>0</v>
-      </c>
+      <c r="BB236" t="inlineStr"/>
+      <c r="BC236" t="inlineStr"/>
+      <c r="BD236" t="inlineStr"/>
+      <c r="BE236" t="inlineStr"/>
       <c r="BF236" t="inlineStr"/>
       <c r="BG236" t="inlineStr"/>
       <c r="BH236" t="inlineStr"/>
@@ -36306,18 +35640,10 @@
       <c r="CJ236" t="inlineStr"/>
       <c r="CK236" t="inlineStr"/>
       <c r="CL236" t="inlineStr"/>
-      <c r="CM236" t="n">
-        <v>0</v>
-      </c>
-      <c r="CN236" t="n">
-        <v>0</v>
-      </c>
-      <c r="CO236" t="n">
-        <v>0</v>
-      </c>
-      <c r="CP236" t="n">
-        <v>1252.4</v>
-      </c>
+      <c r="CM236" t="inlineStr"/>
+      <c r="CN236" t="inlineStr"/>
+      <c r="CO236" t="inlineStr"/>
+      <c r="CP236" t="inlineStr"/>
     </row>
     <row r="237">
       <c r="A237" t="n">
@@ -36422,18 +35748,10 @@
         <v>2004</v>
       </c>
       <c r="BB237" t="inlineStr"/>
-      <c r="BC237" t="n">
-        <v>97.33</v>
-      </c>
-      <c r="BD237" t="n">
-        <v>119.38</v>
-      </c>
-      <c r="BE237" t="n">
-        <v>58.05</v>
-      </c>
-      <c r="BF237" t="n">
-        <v>79.31</v>
-      </c>
+      <c r="BC237" t="inlineStr"/>
+      <c r="BD237" t="inlineStr"/>
+      <c r="BE237" t="inlineStr"/>
+      <c r="BF237" t="inlineStr"/>
       <c r="BG237" t="inlineStr"/>
       <c r="BH237" t="inlineStr"/>
       <c r="BI237" t="inlineStr"/>
@@ -36466,18 +35784,10 @@
       <c r="CJ237" t="inlineStr"/>
       <c r="CK237" t="inlineStr"/>
       <c r="CL237" t="inlineStr"/>
-      <c r="CM237" t="n">
-        <v>98.02</v>
-      </c>
-      <c r="CN237" t="n">
-        <v>87.29000000000001</v>
-      </c>
-      <c r="CO237" t="n">
-        <v>163.84</v>
-      </c>
-      <c r="CP237" t="n">
-        <v>134.22</v>
-      </c>
+      <c r="CM237" t="inlineStr"/>
+      <c r="CN237" t="inlineStr"/>
+      <c r="CO237" t="inlineStr"/>
+      <c r="CP237" t="inlineStr"/>
     </row>
     <row r="238">
       <c r="A238" t="n">
@@ -36582,18 +35892,10 @@
         <v>2004</v>
       </c>
       <c r="BB238" t="inlineStr"/>
-      <c r="BC238" t="n">
-        <v>38.08</v>
-      </c>
-      <c r="BD238" t="n">
-        <v>46.19</v>
-      </c>
-      <c r="BE238" t="n">
-        <v>66.56999999999999</v>
-      </c>
-      <c r="BF238" t="n">
-        <v>84.64</v>
-      </c>
+      <c r="BC238" t="inlineStr"/>
+      <c r="BD238" t="inlineStr"/>
+      <c r="BE238" t="inlineStr"/>
+      <c r="BF238" t="inlineStr"/>
       <c r="BG238" t="inlineStr"/>
       <c r="BH238" t="inlineStr"/>
       <c r="BI238" t="inlineStr"/>
@@ -36626,18 +35928,10 @@
       <c r="CJ238" t="inlineStr"/>
       <c r="CK238" t="inlineStr"/>
       <c r="CL238" t="inlineStr"/>
-      <c r="CM238" t="n">
-        <v>78.88</v>
-      </c>
-      <c r="CN238" t="n">
-        <v>83.89</v>
-      </c>
-      <c r="CO238" t="n">
-        <v>101.26</v>
-      </c>
-      <c r="CP238" t="n">
-        <v>108.05</v>
-      </c>
+      <c r="CM238" t="inlineStr"/>
+      <c r="CN238" t="inlineStr"/>
+      <c r="CO238" t="inlineStr"/>
+      <c r="CP238" t="inlineStr"/>
     </row>
     <row r="239">
       <c r="A239" t="n">
@@ -36742,18 +36036,10 @@
         <v>2004</v>
       </c>
       <c r="BB239" t="inlineStr"/>
-      <c r="BC239" t="n">
-        <v>70.97</v>
-      </c>
-      <c r="BD239" t="n">
-        <v>67.62</v>
-      </c>
-      <c r="BE239" t="n">
-        <v>63.14</v>
-      </c>
-      <c r="BF239" t="n">
-        <v>61.27</v>
-      </c>
+      <c r="BC239" t="inlineStr"/>
+      <c r="BD239" t="inlineStr"/>
+      <c r="BE239" t="inlineStr"/>
+      <c r="BF239" t="inlineStr"/>
       <c r="BG239" t="inlineStr"/>
       <c r="BH239" t="inlineStr"/>
       <c r="BI239" t="inlineStr"/>
@@ -36786,18 +36072,10 @@
       <c r="CJ239" t="inlineStr"/>
       <c r="CK239" t="inlineStr"/>
       <c r="CL239" t="inlineStr"/>
-      <c r="CM239" t="n">
-        <v>36.2</v>
-      </c>
-      <c r="CN239" t="n">
-        <v>51.56</v>
-      </c>
-      <c r="CO239" t="n">
-        <v>38.99</v>
-      </c>
-      <c r="CP239" t="n">
-        <v>36.92</v>
-      </c>
+      <c r="CM239" t="inlineStr"/>
+      <c r="CN239" t="inlineStr"/>
+      <c r="CO239" t="inlineStr"/>
+      <c r="CP239" t="inlineStr"/>
     </row>
     <row r="240">
       <c r="A240" t="n">
@@ -36902,18 +36180,10 @@
         <v>2004</v>
       </c>
       <c r="BB240" t="inlineStr"/>
-      <c r="BC240" t="n">
-        <v>88.03</v>
-      </c>
-      <c r="BD240" t="n">
-        <v>89.59999999999999</v>
-      </c>
-      <c r="BE240" t="n">
-        <v>67.45</v>
-      </c>
-      <c r="BF240" t="n">
-        <v>71.3</v>
-      </c>
+      <c r="BC240" t="inlineStr"/>
+      <c r="BD240" t="inlineStr"/>
+      <c r="BE240" t="inlineStr"/>
+      <c r="BF240" t="inlineStr"/>
       <c r="BG240" t="inlineStr"/>
       <c r="BH240" t="inlineStr"/>
       <c r="BI240" t="inlineStr"/>
@@ -36946,18 +36216,10 @@
       <c r="CJ240" t="inlineStr"/>
       <c r="CK240" t="inlineStr"/>
       <c r="CL240" t="inlineStr"/>
-      <c r="CM240" t="n">
-        <v>67.76000000000001</v>
-      </c>
-      <c r="CN240" t="n">
-        <v>71.62</v>
-      </c>
-      <c r="CO240" t="n">
-        <v>60.81</v>
-      </c>
-      <c r="CP240" t="n">
-        <v>60.99</v>
-      </c>
+      <c r="CM240" t="inlineStr"/>
+      <c r="CN240" t="inlineStr"/>
+      <c r="CO240" t="inlineStr"/>
+      <c r="CP240" t="inlineStr"/>
     </row>
     <row r="241">
       <c r="A241" t="n">
@@ -37059,18 +36321,10 @@
       <c r="BA241" t="n">
         <v>2004</v>
       </c>
-      <c r="BB241" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC241" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD241" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="BE241" t="n">
-        <v>2772.36</v>
-      </c>
+      <c r="BB241" t="inlineStr"/>
+      <c r="BC241" t="inlineStr"/>
+      <c r="BD241" t="inlineStr"/>
+      <c r="BE241" t="inlineStr"/>
       <c r="BF241" t="inlineStr"/>
       <c r="BG241" t="inlineStr"/>
       <c r="BH241" t="inlineStr"/>
@@ -37104,18 +36358,10 @@
       <c r="CJ241" t="inlineStr"/>
       <c r="CK241" t="inlineStr"/>
       <c r="CL241" t="inlineStr"/>
-      <c r="CM241" t="n">
-        <v>2772.36</v>
-      </c>
-      <c r="CN241" t="n">
-        <v>2300.21</v>
-      </c>
-      <c r="CO241" t="n">
-        <v>2093.87</v>
-      </c>
-      <c r="CP241" t="n">
-        <v>2047.32</v>
-      </c>
+      <c r="CM241" t="inlineStr"/>
+      <c r="CN241" t="inlineStr"/>
+      <c r="CO241" t="inlineStr"/>
+      <c r="CP241" t="inlineStr"/>
     </row>
     <row r="242">
       <c r="A242" t="n">
@@ -37555,18 +36801,10 @@
       </c>
       <c r="BB244" t="inlineStr"/>
       <c r="BC244" t="inlineStr"/>
-      <c r="BD244" t="n">
-        <v>2569.36</v>
-      </c>
-      <c r="BE244" t="n">
-        <v>2339.92</v>
-      </c>
-      <c r="BF244" t="n">
-        <v>1671.67</v>
-      </c>
-      <c r="BG244" t="n">
-        <v>1677.95</v>
-      </c>
+      <c r="BD244" t="inlineStr"/>
+      <c r="BE244" t="inlineStr"/>
+      <c r="BF244" t="inlineStr"/>
+      <c r="BG244" t="inlineStr"/>
       <c r="BH244" t="inlineStr"/>
       <c r="BI244" t="inlineStr"/>
       <c r="BJ244" t="inlineStr"/>
@@ -37598,18 +36836,10 @@
       <c r="CJ244" t="inlineStr"/>
       <c r="CK244" t="inlineStr"/>
       <c r="CL244" t="inlineStr"/>
-      <c r="CM244" t="n">
-        <v>1615.54</v>
-      </c>
-      <c r="CN244" t="n">
-        <v>1635.41</v>
-      </c>
-      <c r="CO244" t="n">
-        <v>1642.23</v>
-      </c>
-      <c r="CP244" t="n">
-        <v>1615.78</v>
-      </c>
+      <c r="CM244" t="inlineStr"/>
+      <c r="CN244" t="inlineStr"/>
+      <c r="CO244" t="inlineStr"/>
+      <c r="CP244" t="inlineStr"/>
     </row>
     <row r="245">
       <c r="A245" t="n">
@@ -38011,30 +37241,14 @@
       <c r="BA247" t="n">
         <v>2008</v>
       </c>
-      <c r="BB247" t="n">
-        <v>314.31</v>
-      </c>
-      <c r="BC247" t="n">
-        <v>78.77</v>
-      </c>
-      <c r="BD247" t="n">
-        <v>101.77</v>
-      </c>
-      <c r="BE247" t="n">
-        <v>115.74</v>
-      </c>
-      <c r="BF247" t="n">
-        <v>156.84</v>
-      </c>
-      <c r="BG247" t="n">
-        <v>261.15</v>
-      </c>
-      <c r="BH247" t="n">
-        <v>341.18</v>
-      </c>
-      <c r="BI247" t="n">
-        <v>184.29</v>
-      </c>
+      <c r="BB247" t="inlineStr"/>
+      <c r="BC247" t="inlineStr"/>
+      <c r="BD247" t="inlineStr"/>
+      <c r="BE247" t="inlineStr"/>
+      <c r="BF247" t="inlineStr"/>
+      <c r="BG247" t="inlineStr"/>
+      <c r="BH247" t="inlineStr"/>
+      <c r="BI247" t="inlineStr"/>
       <c r="BJ247" t="inlineStr"/>
       <c r="BK247" t="inlineStr"/>
       <c r="BL247" t="inlineStr"/>
@@ -38064,18 +37278,10 @@
       <c r="CJ247" t="inlineStr"/>
       <c r="CK247" t="inlineStr"/>
       <c r="CL247" t="inlineStr"/>
-      <c r="CM247" t="n">
-        <v>186.81</v>
-      </c>
-      <c r="CN247" t="n">
-        <v>218.11</v>
-      </c>
-      <c r="CO247" t="n">
-        <v>330.4</v>
-      </c>
-      <c r="CP247" t="n">
-        <v>324.82</v>
-      </c>
+      <c r="CM247" t="inlineStr"/>
+      <c r="CN247" t="inlineStr"/>
+      <c r="CO247" t="inlineStr"/>
+      <c r="CP247" t="inlineStr"/>
     </row>
     <row r="248">
       <c r="A248" t="n">
@@ -38185,30 +37391,14 @@
       <c r="BA248" t="n">
         <v>2008</v>
       </c>
-      <c r="BB248" t="n">
-        <v>611.62</v>
-      </c>
-      <c r="BC248" t="n">
-        <v>2669.68</v>
-      </c>
-      <c r="BD248" t="n">
-        <v>2675.88</v>
-      </c>
-      <c r="BE248" t="n">
-        <v>2753.2</v>
-      </c>
-      <c r="BF248" t="n">
-        <v>2771.46</v>
-      </c>
-      <c r="BG248" t="n">
-        <v>2758.94</v>
-      </c>
-      <c r="BH248" t="n">
-        <v>2784.32</v>
-      </c>
-      <c r="BI248" t="n">
-        <v>2741.65</v>
-      </c>
+      <c r="BB248" t="inlineStr"/>
+      <c r="BC248" t="inlineStr"/>
+      <c r="BD248" t="inlineStr"/>
+      <c r="BE248" t="inlineStr"/>
+      <c r="BF248" t="inlineStr"/>
+      <c r="BG248" t="inlineStr"/>
+      <c r="BH248" t="inlineStr"/>
+      <c r="BI248" t="inlineStr"/>
       <c r="BJ248" t="inlineStr"/>
       <c r="BK248" t="inlineStr"/>
       <c r="BL248" t="inlineStr"/>
@@ -38238,18 +37428,10 @@
       <c r="CJ248" t="inlineStr"/>
       <c r="CK248" t="inlineStr"/>
       <c r="CL248" t="inlineStr"/>
-      <c r="CM248" t="n">
-        <v>2796</v>
-      </c>
-      <c r="CN248" t="n">
-        <v>2060.65</v>
-      </c>
-      <c r="CO248" t="n">
-        <v>2066.15</v>
-      </c>
-      <c r="CP248" t="n">
-        <v>2088.03</v>
-      </c>
+      <c r="CM248" t="inlineStr"/>
+      <c r="CN248" t="inlineStr"/>
+      <c r="CO248" t="inlineStr"/>
+      <c r="CP248" t="inlineStr"/>
     </row>
     <row r="249">
       <c r="A249" t="n">
@@ -38359,30 +37541,14 @@
       <c r="BA249" t="n">
         <v>2008</v>
       </c>
-      <c r="BB249" t="n">
-        <v>816.38</v>
-      </c>
-      <c r="BC249" t="n">
-        <v>891.54</v>
-      </c>
-      <c r="BD249" t="n">
-        <v>854.04</v>
-      </c>
-      <c r="BE249" t="n">
-        <v>953.8</v>
-      </c>
-      <c r="BF249" t="n">
-        <v>677.98</v>
-      </c>
-      <c r="BG249" t="n">
-        <v>464.45</v>
-      </c>
-      <c r="BH249" t="n">
-        <v>342.5</v>
-      </c>
-      <c r="BI249" t="n">
-        <v>50.06</v>
-      </c>
+      <c r="BB249" t="inlineStr"/>
+      <c r="BC249" t="inlineStr"/>
+      <c r="BD249" t="inlineStr"/>
+      <c r="BE249" t="inlineStr"/>
+      <c r="BF249" t="inlineStr"/>
+      <c r="BG249" t="inlineStr"/>
+      <c r="BH249" t="inlineStr"/>
+      <c r="BI249" t="inlineStr"/>
       <c r="BJ249" t="inlineStr"/>
       <c r="BK249" t="inlineStr"/>
       <c r="BL249" t="inlineStr"/>
@@ -38412,18 +37578,10 @@
       <c r="CJ249" t="inlineStr"/>
       <c r="CK249" t="inlineStr"/>
       <c r="CL249" t="inlineStr"/>
-      <c r="CM249" t="n">
-        <v>79.13</v>
-      </c>
-      <c r="CN249" t="n">
-        <v>78.37</v>
-      </c>
-      <c r="CO249" t="n">
-        <v>148.47</v>
-      </c>
-      <c r="CP249" t="n">
-        <v>365.7</v>
-      </c>
+      <c r="CM249" t="inlineStr"/>
+      <c r="CN249" t="inlineStr"/>
+      <c r="CO249" t="inlineStr"/>
+      <c r="CP249" t="inlineStr"/>
     </row>
     <row r="250">
       <c r="A250" t="n">
@@ -38679,30 +37837,14 @@
       <c r="BA251" t="n">
         <v>2008</v>
       </c>
-      <c r="BB251" t="n">
-        <v>2946.44</v>
-      </c>
-      <c r="BC251" t="n">
-        <v>2747.86</v>
-      </c>
-      <c r="BD251" t="n">
-        <v>2705</v>
-      </c>
-      <c r="BE251" t="n">
-        <v>3139.8</v>
-      </c>
-      <c r="BF251" t="n">
-        <v>3233.78</v>
-      </c>
-      <c r="BG251" t="n">
-        <v>3233.45</v>
-      </c>
-      <c r="BH251" t="n">
-        <v>3232.41</v>
-      </c>
-      <c r="BI251" t="n">
-        <v>3288.72</v>
-      </c>
+      <c r="BB251" t="inlineStr"/>
+      <c r="BC251" t="inlineStr"/>
+      <c r="BD251" t="inlineStr"/>
+      <c r="BE251" t="inlineStr"/>
+      <c r="BF251" t="inlineStr"/>
+      <c r="BG251" t="inlineStr"/>
+      <c r="BH251" t="inlineStr"/>
+      <c r="BI251" t="inlineStr"/>
       <c r="BJ251" t="inlineStr"/>
       <c r="BK251" t="inlineStr"/>
       <c r="BL251" t="inlineStr"/>
@@ -38732,18 +37874,10 @@
       <c r="CJ251" t="inlineStr"/>
       <c r="CK251" t="inlineStr"/>
       <c r="CL251" t="inlineStr"/>
-      <c r="CM251" t="n">
-        <v>3245.11</v>
-      </c>
-      <c r="CN251" t="n">
-        <v>3136.1</v>
-      </c>
-      <c r="CO251" t="n">
-        <v>3441.98</v>
-      </c>
-      <c r="CP251" t="n">
-        <v>2984.12</v>
-      </c>
+      <c r="CM251" t="inlineStr"/>
+      <c r="CN251" t="inlineStr"/>
+      <c r="CO251" t="inlineStr"/>
+      <c r="CP251" t="inlineStr"/>
     </row>
     <row r="252">
       <c r="A252" t="n">
@@ -38849,24 +37983,12 @@
       <c r="BA252" t="n">
         <v>2008</v>
       </c>
-      <c r="BB252" t="n">
-        <v>5016.63</v>
-      </c>
-      <c r="BC252" t="n">
-        <v>108.53</v>
-      </c>
-      <c r="BD252" t="n">
-        <v>148.96</v>
-      </c>
-      <c r="BE252" t="n">
-        <v>83.06</v>
-      </c>
-      <c r="BF252" t="n">
-        <v>81.22</v>
-      </c>
-      <c r="BG252" t="n">
-        <v>85.47</v>
-      </c>
+      <c r="BB252" t="inlineStr"/>
+      <c r="BC252" t="inlineStr"/>
+      <c r="BD252" t="inlineStr"/>
+      <c r="BE252" t="inlineStr"/>
+      <c r="BF252" t="inlineStr"/>
+      <c r="BG252" t="inlineStr"/>
       <c r="BH252" t="inlineStr"/>
       <c r="BI252" t="inlineStr"/>
       <c r="BJ252" t="inlineStr"/>
@@ -38898,18 +38020,10 @@
       <c r="CJ252" t="inlineStr"/>
       <c r="CK252" t="inlineStr"/>
       <c r="CL252" t="inlineStr"/>
-      <c r="CM252" t="n">
-        <v>75.92</v>
-      </c>
-      <c r="CN252" t="n">
-        <v>102.93</v>
-      </c>
-      <c r="CO252" t="n">
-        <v>117.44</v>
-      </c>
-      <c r="CP252" t="n">
-        <v>44.15</v>
-      </c>
+      <c r="CM252" t="inlineStr"/>
+      <c r="CN252" t="inlineStr"/>
+      <c r="CO252" t="inlineStr"/>
+      <c r="CP252" t="inlineStr"/>
     </row>
     <row r="253">
       <c r="A253" t="n">
@@ -39015,24 +38129,12 @@
       <c r="BA253" t="n">
         <v>2008</v>
       </c>
-      <c r="BB253" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC253" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD253" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE253" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF253" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG253" t="n">
-        <v>3972.97</v>
-      </c>
+      <c r="BB253" t="inlineStr"/>
+      <c r="BC253" t="inlineStr"/>
+      <c r="BD253" t="inlineStr"/>
+      <c r="BE253" t="inlineStr"/>
+      <c r="BF253" t="inlineStr"/>
+      <c r="BG253" t="inlineStr"/>
       <c r="BH253" t="inlineStr"/>
       <c r="BI253" t="inlineStr"/>
       <c r="BJ253" t="inlineStr"/>
@@ -39064,18 +38166,10 @@
       <c r="CJ253" t="inlineStr"/>
       <c r="CK253" t="inlineStr"/>
       <c r="CL253" t="inlineStr"/>
-      <c r="CM253" t="n">
-        <v>2516.92</v>
-      </c>
-      <c r="CN253" t="n">
-        <v>2516.93</v>
-      </c>
-      <c r="CO253" t="n">
-        <v>1833.72</v>
-      </c>
-      <c r="CP253" t="n">
-        <v>1611.41</v>
-      </c>
+      <c r="CM253" t="inlineStr"/>
+      <c r="CN253" t="inlineStr"/>
+      <c r="CO253" t="inlineStr"/>
+      <c r="CP253" t="inlineStr"/>
     </row>
     <row r="254">
       <c r="A254" t="n">
@@ -39181,24 +38275,12 @@
       <c r="BA254" t="n">
         <v>2008</v>
       </c>
-      <c r="BB254" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC254" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD254" t="n">
-        <v>1163.7</v>
-      </c>
-      <c r="BE254" t="n">
-        <v>801.17</v>
-      </c>
-      <c r="BF254" t="n">
-        <v>309.06</v>
-      </c>
-      <c r="BG254" t="n">
-        <v>222.31</v>
-      </c>
+      <c r="BB254" t="inlineStr"/>
+      <c r="BC254" t="inlineStr"/>
+      <c r="BD254" t="inlineStr"/>
+      <c r="BE254" t="inlineStr"/>
+      <c r="BF254" t="inlineStr"/>
+      <c r="BG254" t="inlineStr"/>
       <c r="BH254" t="inlineStr"/>
       <c r="BI254" t="inlineStr"/>
       <c r="BJ254" t="inlineStr"/>
@@ -39230,18 +38312,10 @@
       <c r="CJ254" t="inlineStr"/>
       <c r="CK254" t="inlineStr"/>
       <c r="CL254" t="inlineStr"/>
-      <c r="CM254" t="n">
-        <v>226.14</v>
-      </c>
-      <c r="CN254" t="n">
-        <v>161.22</v>
-      </c>
-      <c r="CO254" t="n">
-        <v>117.24</v>
-      </c>
-      <c r="CP254" t="n">
-        <v>104.13</v>
-      </c>
+      <c r="CM254" t="inlineStr"/>
+      <c r="CN254" t="inlineStr"/>
+      <c r="CO254" t="inlineStr"/>
+      <c r="CP254" t="inlineStr"/>
     </row>
     <row r="255">
       <c r="A255" t="n">
@@ -39347,24 +38421,12 @@
       <c r="BA255" t="n">
         <v>2008</v>
       </c>
-      <c r="BB255" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC255" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD255" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE255" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF255" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG255" t="n">
-        <v>0</v>
-      </c>
+      <c r="BB255" t="inlineStr"/>
+      <c r="BC255" t="inlineStr"/>
+      <c r="BD255" t="inlineStr"/>
+      <c r="BE255" t="inlineStr"/>
+      <c r="BF255" t="inlineStr"/>
+      <c r="BG255" t="inlineStr"/>
       <c r="BH255" t="inlineStr"/>
       <c r="BI255" t="inlineStr"/>
       <c r="BJ255" t="inlineStr"/>
@@ -39396,18 +38458,10 @@
       <c r="CJ255" t="inlineStr"/>
       <c r="CK255" t="inlineStr"/>
       <c r="CL255" t="inlineStr"/>
-      <c r="CM255" t="n">
-        <v>0</v>
-      </c>
-      <c r="CN255" t="n">
-        <v>144.48</v>
-      </c>
-      <c r="CO255" t="n">
-        <v>168.97</v>
-      </c>
-      <c r="CP255" t="n">
-        <v>126.17</v>
-      </c>
+      <c r="CM255" t="inlineStr"/>
+      <c r="CN255" t="inlineStr"/>
+      <c r="CO255" t="inlineStr"/>
+      <c r="CP255" t="inlineStr"/>
     </row>
     <row r="256">
       <c r="A256" t="n">
@@ -39655,24 +38709,12 @@
       <c r="BA257" t="n">
         <v>2008</v>
       </c>
-      <c r="BB257" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC257" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD257" t="n">
-        <v>2.32</v>
-      </c>
-      <c r="BE257" t="n">
-        <v>347.57</v>
-      </c>
-      <c r="BF257" t="n">
-        <v>124.7</v>
-      </c>
-      <c r="BG257" t="n">
-        <v>86.34</v>
-      </c>
+      <c r="BB257" t="inlineStr"/>
+      <c r="BC257" t="inlineStr"/>
+      <c r="BD257" t="inlineStr"/>
+      <c r="BE257" t="inlineStr"/>
+      <c r="BF257" t="inlineStr"/>
+      <c r="BG257" t="inlineStr"/>
       <c r="BH257" t="inlineStr"/>
       <c r="BI257" t="inlineStr"/>
       <c r="BJ257" t="inlineStr"/>
@@ -39704,18 +38746,10 @@
       <c r="CJ257" t="inlineStr"/>
       <c r="CK257" t="inlineStr"/>
       <c r="CL257" t="inlineStr"/>
-      <c r="CM257" t="n">
-        <v>115.38</v>
-      </c>
-      <c r="CN257" t="n">
-        <v>120.06</v>
-      </c>
-      <c r="CO257" t="n">
-        <v>112.41</v>
-      </c>
-      <c r="CP257" t="n">
-        <v>96.59999999999999</v>
-      </c>
+      <c r="CM257" t="inlineStr"/>
+      <c r="CN257" t="inlineStr"/>
+      <c r="CO257" t="inlineStr"/>
+      <c r="CP257" t="inlineStr"/>
     </row>
     <row r="258">
       <c r="A258" t="n">
@@ -40541,15 +39575,9 @@
       <c r="BG262" t="inlineStr"/>
       <c r="BH262" t="inlineStr"/>
       <c r="BI262" t="inlineStr"/>
-      <c r="BJ262" t="n">
-        <v>89.28</v>
-      </c>
-      <c r="BK262" t="n">
-        <v>95.84</v>
-      </c>
-      <c r="BL262" t="n">
-        <v>85.98</v>
-      </c>
+      <c r="BJ262" t="inlineStr"/>
+      <c r="BK262" t="inlineStr"/>
+      <c r="BL262" t="inlineStr"/>
       <c r="BM262" t="inlineStr"/>
       <c r="BN262" t="inlineStr"/>
       <c r="BO262" t="inlineStr"/>
@@ -40576,18 +39604,10 @@
       <c r="CJ262" t="inlineStr"/>
       <c r="CK262" t="inlineStr"/>
       <c r="CL262" t="inlineStr"/>
-      <c r="CM262" t="n">
-        <v>197.01</v>
-      </c>
-      <c r="CN262" t="n">
-        <v>205.89</v>
-      </c>
-      <c r="CO262" t="n">
-        <v>175.99</v>
-      </c>
-      <c r="CP262" t="n">
-        <v>190.2</v>
-      </c>
+      <c r="CM262" t="inlineStr"/>
+      <c r="CN262" t="inlineStr"/>
+      <c r="CO262" t="inlineStr"/>
+      <c r="CP262" t="inlineStr"/>
     </row>
     <row r="263">
       <c r="A263" t="n">
@@ -40720,15 +39740,9 @@
       <c r="BJ263" t="inlineStr"/>
       <c r="BK263" t="inlineStr"/>
       <c r="BL263" t="inlineStr"/>
-      <c r="BM263" t="n">
-        <v>136.25</v>
-      </c>
-      <c r="BN263" t="n">
-        <v>131.73</v>
-      </c>
-      <c r="BO263" t="n">
-        <v>128.16</v>
-      </c>
+      <c r="BM263" t="inlineStr"/>
+      <c r="BN263" t="inlineStr"/>
+      <c r="BO263" t="inlineStr"/>
       <c r="BP263" t="inlineStr"/>
       <c r="BQ263" t="inlineStr"/>
       <c r="BR263" t="inlineStr"/>
@@ -40752,18 +39766,10 @@
       <c r="CJ263" t="inlineStr"/>
       <c r="CK263" t="inlineStr"/>
       <c r="CL263" t="inlineStr"/>
-      <c r="CM263" t="n">
-        <v>153.64</v>
-      </c>
-      <c r="CN263" t="n">
-        <v>123.94</v>
-      </c>
-      <c r="CO263" t="n">
-        <v>86.31</v>
-      </c>
-      <c r="CP263" t="n">
-        <v>169.89</v>
-      </c>
+      <c r="CM263" t="inlineStr"/>
+      <c r="CN263" t="inlineStr"/>
+      <c r="CO263" t="inlineStr"/>
+      <c r="CP263" t="inlineStr"/>
     </row>
     <row r="264">
       <c r="A264" t="n">
@@ -40865,18 +39871,10 @@
       <c r="BA264" t="n">
         <v>2006</v>
       </c>
-      <c r="BB264" t="n">
-        <v>687.84</v>
-      </c>
-      <c r="BC264" t="n">
-        <v>414.02</v>
-      </c>
-      <c r="BD264" t="n">
-        <v>883.98</v>
-      </c>
-      <c r="BE264" t="n">
-        <v>277.19</v>
-      </c>
+      <c r="BB264" t="inlineStr"/>
+      <c r="BC264" t="inlineStr"/>
+      <c r="BD264" t="inlineStr"/>
+      <c r="BE264" t="inlineStr"/>
       <c r="BF264" t="inlineStr"/>
       <c r="BG264" t="inlineStr"/>
       <c r="BH264" t="inlineStr"/>
@@ -40910,18 +39908,10 @@
       <c r="CJ264" t="inlineStr"/>
       <c r="CK264" t="inlineStr"/>
       <c r="CL264" t="inlineStr"/>
-      <c r="CM264" t="n">
-        <v>277.19</v>
-      </c>
-      <c r="CN264" t="n">
-        <v>231.15</v>
-      </c>
-      <c r="CO264" t="n">
-        <v>227.02</v>
-      </c>
-      <c r="CP264" t="n">
-        <v>139.38</v>
-      </c>
+      <c r="CM264" t="inlineStr"/>
+      <c r="CN264" t="inlineStr"/>
+      <c r="CO264" t="inlineStr"/>
+      <c r="CP264" t="inlineStr"/>
     </row>
     <row r="265">
       <c r="A265" t="n">
@@ -41185,21 +40175,11 @@
       <c r="BC266" t="inlineStr"/>
       <c r="BD266" t="inlineStr"/>
       <c r="BE266" t="inlineStr"/>
-      <c r="BF266" t="n">
-        <v>62.53</v>
-      </c>
-      <c r="BG266" t="n">
-        <v>57.25</v>
-      </c>
-      <c r="BH266" t="n">
-        <v>126.46</v>
-      </c>
-      <c r="BI266" t="n">
-        <v>280.45</v>
-      </c>
-      <c r="BJ266" t="n">
-        <v>165.24</v>
-      </c>
+      <c r="BF266" t="inlineStr"/>
+      <c r="BG266" t="inlineStr"/>
+      <c r="BH266" t="inlineStr"/>
+      <c r="BI266" t="inlineStr"/>
+      <c r="BJ266" t="inlineStr"/>
       <c r="BK266" t="inlineStr"/>
       <c r="BL266" t="inlineStr"/>
       <c r="BM266" t="inlineStr"/>
@@ -41228,18 +40208,10 @@
       <c r="CJ266" t="inlineStr"/>
       <c r="CK266" t="inlineStr"/>
       <c r="CL266" t="inlineStr"/>
-      <c r="CM266" t="n">
-        <v>150.74</v>
-      </c>
-      <c r="CN266" t="n">
-        <v>162.87</v>
-      </c>
-      <c r="CO266" t="n">
-        <v>152.63</v>
-      </c>
-      <c r="CP266" t="n">
-        <v>139.77</v>
-      </c>
+      <c r="CM266" t="inlineStr"/>
+      <c r="CN266" t="inlineStr"/>
+      <c r="CO266" t="inlineStr"/>
+      <c r="CP266" t="inlineStr"/>
     </row>
     <row r="267">
       <c r="A267" t="n">
@@ -41355,21 +40327,11 @@
       <c r="BC267" t="inlineStr"/>
       <c r="BD267" t="inlineStr"/>
       <c r="BE267" t="inlineStr"/>
-      <c r="BF267" t="n">
-        <v>663.85</v>
-      </c>
-      <c r="BG267" t="n">
-        <v>341.79</v>
-      </c>
-      <c r="BH267" t="n">
-        <v>341.94</v>
-      </c>
-      <c r="BI267" t="n">
-        <v>342.01</v>
-      </c>
-      <c r="BJ267" t="n">
-        <v>1056.26</v>
-      </c>
+      <c r="BF267" t="inlineStr"/>
+      <c r="BG267" t="inlineStr"/>
+      <c r="BH267" t="inlineStr"/>
+      <c r="BI267" t="inlineStr"/>
+      <c r="BJ267" t="inlineStr"/>
       <c r="BK267" t="inlineStr"/>
       <c r="BL267" t="inlineStr"/>
       <c r="BM267" t="inlineStr"/>
@@ -41398,18 +40360,10 @@
       <c r="CJ267" t="inlineStr"/>
       <c r="CK267" t="inlineStr"/>
       <c r="CL267" t="inlineStr"/>
-      <c r="CM267" t="n">
-        <v>1056.47</v>
-      </c>
-      <c r="CN267" t="n">
-        <v>1251.03</v>
-      </c>
-      <c r="CO267" t="n">
-        <v>109.76</v>
-      </c>
-      <c r="CP267" t="n">
-        <v>1294.8</v>
-      </c>
+      <c r="CM267" t="inlineStr"/>
+      <c r="CN267" t="inlineStr"/>
+      <c r="CO267" t="inlineStr"/>
+      <c r="CP267" t="inlineStr"/>
     </row>
     <row r="268">
       <c r="A268" t="n">
@@ -41513,21 +40467,11 @@
       <c r="BA268" t="n">
         <v>2005</v>
       </c>
-      <c r="BB268" t="n">
-        <v>4225.22</v>
-      </c>
-      <c r="BC268" t="n">
-        <v>3983.75</v>
-      </c>
-      <c r="BD268" t="n">
-        <v>4008.82</v>
-      </c>
-      <c r="BE268" t="n">
-        <v>4027.78</v>
-      </c>
-      <c r="BF268" t="n">
-        <v>4008.03</v>
-      </c>
+      <c r="BB268" t="inlineStr"/>
+      <c r="BC268" t="inlineStr"/>
+      <c r="BD268" t="inlineStr"/>
+      <c r="BE268" t="inlineStr"/>
+      <c r="BF268" t="inlineStr"/>
       <c r="BG268" t="inlineStr"/>
       <c r="BH268" t="inlineStr"/>
       <c r="BI268" t="inlineStr"/>
@@ -41560,18 +40504,10 @@
       <c r="CJ268" t="inlineStr"/>
       <c r="CK268" t="inlineStr"/>
       <c r="CL268" t="inlineStr"/>
-      <c r="CM268" t="n">
-        <v>7.18</v>
-      </c>
-      <c r="CN268" t="n">
-        <v>3973.15</v>
-      </c>
-      <c r="CO268" t="n">
-        <v>3972.35</v>
-      </c>
-      <c r="CP268" t="n">
-        <v>4023.12</v>
-      </c>
+      <c r="CM268" t="inlineStr"/>
+      <c r="CN268" t="inlineStr"/>
+      <c r="CO268" t="inlineStr"/>
+      <c r="CP268" t="inlineStr"/>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -41841,18 +40777,10 @@
       <c r="BA270" t="n">
         <v>2003</v>
       </c>
-      <c r="BB270" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC270" t="n">
-        <v>264.81</v>
-      </c>
-      <c r="BD270" t="n">
-        <v>916409.73</v>
-      </c>
-      <c r="BE270" t="n">
-        <v>162045.59</v>
-      </c>
+      <c r="BB270" t="inlineStr"/>
+      <c r="BC270" t="inlineStr"/>
+      <c r="BD270" t="inlineStr"/>
+      <c r="BE270" t="inlineStr"/>
       <c r="BF270" t="inlineStr"/>
       <c r="BG270" t="inlineStr"/>
       <c r="BH270" t="inlineStr"/>
@@ -41886,18 +40814,10 @@
       <c r="CJ270" t="inlineStr"/>
       <c r="CK270" t="inlineStr"/>
       <c r="CL270" t="inlineStr"/>
-      <c r="CM270" t="n">
-        <v>162045.59</v>
-      </c>
-      <c r="CN270" t="n">
-        <v>40.04</v>
-      </c>
-      <c r="CO270" t="n">
-        <v>63.64</v>
-      </c>
-      <c r="CP270" t="n">
-        <v>9301.01</v>
-      </c>
+      <c r="CM270" t="inlineStr"/>
+      <c r="CN270" t="inlineStr"/>
+      <c r="CO270" t="inlineStr"/>
+      <c r="CP270" t="inlineStr"/>
     </row>
     <row r="271">
       <c r="A271" t="n">
@@ -42283,27 +41203,13 @@
       <c r="BA273" t="n">
         <v>2008</v>
       </c>
-      <c r="BB273" t="n">
-        <v>0</v>
-      </c>
-      <c r="BC273" t="n">
-        <v>0</v>
-      </c>
-      <c r="BD273" t="n">
-        <v>0</v>
-      </c>
-      <c r="BE273" t="n">
-        <v>0</v>
-      </c>
-      <c r="BF273" t="n">
-        <v>0</v>
-      </c>
-      <c r="BG273" t="n">
-        <v>0</v>
-      </c>
-      <c r="BH273" t="n">
-        <v>0</v>
-      </c>
+      <c r="BB273" t="inlineStr"/>
+      <c r="BC273" t="inlineStr"/>
+      <c r="BD273" t="inlineStr"/>
+      <c r="BE273" t="inlineStr"/>
+      <c r="BF273" t="inlineStr"/>
+      <c r="BG273" t="inlineStr"/>
+      <c r="BH273" t="inlineStr"/>
       <c r="BI273" t="inlineStr"/>
       <c r="BJ273" t="inlineStr"/>
       <c r="BK273" t="inlineStr"/>
@@ -42334,18 +41240,10 @@
       <c r="CJ273" t="inlineStr"/>
       <c r="CK273" t="inlineStr"/>
       <c r="CL273" t="inlineStr"/>
-      <c r="CM273" t="n">
-        <v>6437.72</v>
-      </c>
-      <c r="CN273" t="n">
-        <v>6437.58</v>
-      </c>
-      <c r="CO273" t="n">
-        <v>6372.86</v>
-      </c>
-      <c r="CP273" t="n">
-        <v>1314.5</v>
-      </c>
+      <c r="CM273" t="inlineStr"/>
+      <c r="CN273" t="inlineStr"/>
+      <c r="CO273" t="inlineStr"/>
+      <c r="CP273" t="inlineStr"/>
     </row>
     <row r="274">
       <c r="A274" t="n">
@@ -43487,21 +42385,11 @@
       <c r="BA280" t="n">
         <v>2007</v>
       </c>
-      <c r="BB280" t="n">
-        <v>2596.84</v>
-      </c>
-      <c r="BC280" t="n">
-        <v>2573.26</v>
-      </c>
-      <c r="BD280" t="n">
-        <v>2707.18</v>
-      </c>
-      <c r="BE280" t="n">
-        <v>2709.42</v>
-      </c>
-      <c r="BF280" t="n">
-        <v>2654.34</v>
-      </c>
+      <c r="BB280" t="inlineStr"/>
+      <c r="BC280" t="inlineStr"/>
+      <c r="BD280" t="inlineStr"/>
+      <c r="BE280" t="inlineStr"/>
+      <c r="BF280" t="inlineStr"/>
       <c r="BG280" t="inlineStr"/>
       <c r="BH280" t="inlineStr"/>
       <c r="BI280" t="inlineStr"/>
@@ -43534,18 +42422,10 @@
       <c r="CJ280" t="inlineStr"/>
       <c r="CK280" t="inlineStr"/>
       <c r="CL280" t="inlineStr"/>
-      <c r="CM280" t="n">
-        <v>2704.86</v>
-      </c>
-      <c r="CN280" t="n">
-        <v>2704.89</v>
-      </c>
-      <c r="CO280" t="n">
-        <v>2689.91</v>
-      </c>
-      <c r="CP280" t="n">
-        <v>2690.79</v>
-      </c>
+      <c r="CM280" t="inlineStr"/>
+      <c r="CN280" t="inlineStr"/>
+      <c r="CO280" t="inlineStr"/>
+      <c r="CP280" t="inlineStr"/>
     </row>
     <row r="281">
       <c r="A281" t="n">
@@ -43649,21 +42529,11 @@
       <c r="BA281" t="n">
         <v>2007</v>
       </c>
-      <c r="BB281" t="n">
-        <v>93.66</v>
-      </c>
-      <c r="BC281" t="n">
-        <v>78.51000000000001</v>
-      </c>
-      <c r="BD281" t="n">
-        <v>74.7</v>
-      </c>
-      <c r="BE281" t="n">
-        <v>75.09</v>
-      </c>
-      <c r="BF281" t="n">
-        <v>78.34</v>
-      </c>
+      <c r="BB281" t="inlineStr"/>
+      <c r="BC281" t="inlineStr"/>
+      <c r="BD281" t="inlineStr"/>
+      <c r="BE281" t="inlineStr"/>
+      <c r="BF281" t="inlineStr"/>
       <c r="BG281" t="inlineStr"/>
       <c r="BH281" t="inlineStr"/>
       <c r="BI281" t="inlineStr"/>
@@ -43696,18 +42566,10 @@
       <c r="CJ281" t="inlineStr"/>
       <c r="CK281" t="inlineStr"/>
       <c r="CL281" t="inlineStr"/>
-      <c r="CM281" t="n">
-        <v>74.40000000000001</v>
-      </c>
-      <c r="CN281" t="n">
-        <v>66.73999999999999</v>
-      </c>
-      <c r="CO281" t="n">
-        <v>63.28</v>
-      </c>
-      <c r="CP281" t="n">
-        <v>54.01</v>
-      </c>
+      <c r="CM281" t="inlineStr"/>
+      <c r="CN281" t="inlineStr"/>
+      <c r="CO281" t="inlineStr"/>
+      <c r="CP281" t="inlineStr"/>
     </row>
     <row r="282">
       <c r="A282" t="n">
@@ -43811,21 +42673,11 @@
       <c r="BA282" t="n">
         <v>2007</v>
       </c>
-      <c r="BB282" t="n">
-        <v>92.11</v>
-      </c>
-      <c r="BC282" t="n">
-        <v>104.6</v>
-      </c>
-      <c r="BD282" t="n">
-        <v>101.37</v>
-      </c>
-      <c r="BE282" t="n">
-        <v>116.58</v>
-      </c>
-      <c r="BF282" t="n">
-        <v>108.66</v>
-      </c>
+      <c r="BB282" t="inlineStr"/>
+      <c r="BC282" t="inlineStr"/>
+      <c r="BD282" t="inlineStr"/>
+      <c r="BE282" t="inlineStr"/>
+      <c r="BF282" t="inlineStr"/>
       <c r="BG282" t="inlineStr"/>
       <c r="BH282" t="inlineStr"/>
       <c r="BI282" t="inlineStr"/>
@@ -43858,18 +42710,10 @@
       <c r="CJ282" t="inlineStr"/>
       <c r="CK282" t="inlineStr"/>
       <c r="CL282" t="inlineStr"/>
-      <c r="CM282" t="n">
-        <v>149.84</v>
-      </c>
-      <c r="CN282" t="n">
-        <v>122.21</v>
-      </c>
-      <c r="CO282" t="n">
-        <v>116.99</v>
-      </c>
-      <c r="CP282" t="n">
-        <v>110.29</v>
-      </c>
+      <c r="CM282" t="inlineStr"/>
+      <c r="CN282" t="inlineStr"/>
+      <c r="CO282" t="inlineStr"/>
+      <c r="CP282" t="inlineStr"/>
     </row>
     <row r="283">
       <c r="A283" t="n">
@@ -43973,21 +42817,11 @@
       <c r="BA283" t="n">
         <v>2007</v>
       </c>
-      <c r="BB283" t="n">
-        <v>4.73</v>
-      </c>
-      <c r="BC283" t="n">
-        <v>4.68</v>
-      </c>
-      <c r="BD283" t="n">
-        <v>5.18</v>
-      </c>
-      <c r="BE283" t="n">
-        <v>6.43</v>
-      </c>
-      <c r="BF283" t="n">
-        <v>64.58</v>
-      </c>
+      <c r="BB283" t="inlineStr"/>
+      <c r="BC283" t="inlineStr"/>
+      <c r="BD283" t="inlineStr"/>
+      <c r="BE283" t="inlineStr"/>
+      <c r="BF283" t="inlineStr"/>
       <c r="BG283" t="inlineStr"/>
       <c r="BH283" t="inlineStr"/>
       <c r="BI283" t="inlineStr"/>
@@ -44020,18 +42854,10 @@
       <c r="CJ283" t="inlineStr"/>
       <c r="CK283" t="inlineStr"/>
       <c r="CL283" t="inlineStr"/>
-      <c r="CM283" t="n">
-        <v>28.06</v>
-      </c>
-      <c r="CN283" t="n">
-        <v>62.66</v>
-      </c>
-      <c r="CO283" t="n">
-        <v>2.24</v>
-      </c>
-      <c r="CP283" t="n">
-        <v>2.24</v>
-      </c>
+      <c r="CM283" t="inlineStr"/>
+      <c r="CN283" t="inlineStr"/>
+      <c r="CO283" t="inlineStr"/>
+      <c r="CP283" t="inlineStr"/>
     </row>
     <row r="284">
       <c r="A284" t="n">
@@ -44702,27 +43528,13 @@
         <v>2007</v>
       </c>
       <c r="BB288" t="inlineStr"/>
-      <c r="BC288" t="n">
-        <v>1827.28</v>
-      </c>
-      <c r="BD288" t="n">
-        <v>1827.24</v>
-      </c>
-      <c r="BE288" t="n">
-        <v>1812.3</v>
-      </c>
-      <c r="BF288" t="n">
-        <v>1337.52</v>
-      </c>
-      <c r="BG288" t="n">
-        <v>257.01</v>
-      </c>
-      <c r="BH288" t="n">
-        <v>257.91</v>
-      </c>
-      <c r="BI288" t="n">
-        <v>54.62</v>
-      </c>
+      <c r="BC288" t="inlineStr"/>
+      <c r="BD288" t="inlineStr"/>
+      <c r="BE288" t="inlineStr"/>
+      <c r="BF288" t="inlineStr"/>
+      <c r="BG288" t="inlineStr"/>
+      <c r="BH288" t="inlineStr"/>
+      <c r="BI288" t="inlineStr"/>
       <c r="BJ288" t="inlineStr"/>
       <c r="BK288" t="inlineStr"/>
       <c r="BL288" t="inlineStr"/>
@@ -44752,18 +43564,10 @@
       <c r="CJ288" t="inlineStr"/>
       <c r="CK288" t="inlineStr"/>
       <c r="CL288" t="inlineStr"/>
-      <c r="CM288" t="n">
-        <v>87.06999999999999</v>
-      </c>
-      <c r="CN288" t="n">
-        <v>252.7</v>
-      </c>
-      <c r="CO288" t="n">
-        <v>792.52</v>
-      </c>
-      <c r="CP288" t="n">
-        <v>305.39</v>
-      </c>
+      <c r="CM288" t="inlineStr"/>
+      <c r="CN288" t="inlineStr"/>
+      <c r="CO288" t="inlineStr"/>
+      <c r="CP288" t="inlineStr"/>
     </row>
     <row r="289">
       <c r="A289" t="n">
@@ -45159,24 +43963,12 @@
       <c r="BA291" t="n">
         <v>2010</v>
       </c>
-      <c r="BB291" t="n">
-        <v>429.39</v>
-      </c>
-      <c r="BC291" t="n">
-        <v>509.97</v>
-      </c>
-      <c r="BD291" t="n">
-        <v>555.53</v>
-      </c>
-      <c r="BE291" t="n">
-        <v>580.92</v>
-      </c>
-      <c r="BF291" t="n">
-        <v>451.26</v>
-      </c>
-      <c r="BG291" t="n">
-        <v>561.66</v>
-      </c>
+      <c r="BB291" t="inlineStr"/>
+      <c r="BC291" t="inlineStr"/>
+      <c r="BD291" t="inlineStr"/>
+      <c r="BE291" t="inlineStr"/>
+      <c r="BF291" t="inlineStr"/>
+      <c r="BG291" t="inlineStr"/>
       <c r="BH291" t="inlineStr"/>
       <c r="BI291" t="inlineStr"/>
       <c r="BJ291" t="inlineStr"/>
@@ -45208,18 +44000,10 @@
       <c r="CJ291" t="inlineStr"/>
       <c r="CK291" t="inlineStr"/>
       <c r="CL291" t="inlineStr"/>
-      <c r="CM291" t="n">
-        <v>502.52</v>
-      </c>
-      <c r="CN291" t="n">
-        <v>548.33</v>
-      </c>
-      <c r="CO291" t="n">
-        <v>492.47</v>
-      </c>
-      <c r="CP291" t="n">
-        <v>418.12</v>
-      </c>
+      <c r="CM291" t="inlineStr"/>
+      <c r="CN291" t="inlineStr"/>
+      <c r="CO291" t="inlineStr"/>
+      <c r="CP291" t="inlineStr"/>
     </row>
     <row r="292">
       <c r="A292" t="n">
@@ -45325,24 +44109,12 @@
       <c r="BA292" t="n">
         <v>2010</v>
       </c>
-      <c r="BB292" t="n">
-        <v>79.16</v>
-      </c>
-      <c r="BC292" t="n">
-        <v>62.55</v>
-      </c>
-      <c r="BD292" t="n">
-        <v>32.97</v>
-      </c>
-      <c r="BE292" t="n">
-        <v>28.61</v>
-      </c>
-      <c r="BF292" t="n">
-        <v>26.83</v>
-      </c>
-      <c r="BG292" t="n">
-        <v>23.34</v>
-      </c>
+      <c r="BB292" t="inlineStr"/>
+      <c r="BC292" t="inlineStr"/>
+      <c r="BD292" t="inlineStr"/>
+      <c r="BE292" t="inlineStr"/>
+      <c r="BF292" t="inlineStr"/>
+      <c r="BG292" t="inlineStr"/>
       <c r="BH292" t="inlineStr"/>
       <c r="BI292" t="inlineStr"/>
       <c r="BJ292" t="inlineStr"/>
@@ -45374,18 +44146,10 @@
       <c r="CJ292" t="inlineStr"/>
       <c r="CK292" t="inlineStr"/>
       <c r="CL292" t="inlineStr"/>
-      <c r="CM292" t="n">
-        <v>42.84</v>
-      </c>
-      <c r="CN292" t="n">
-        <v>39.58</v>
-      </c>
-      <c r="CO292" t="n">
-        <v>38.05</v>
-      </c>
-      <c r="CP292" t="n">
-        <v>39.48</v>
-      </c>
+      <c r="CM292" t="inlineStr"/>
+      <c r="CN292" t="inlineStr"/>
+      <c r="CO292" t="inlineStr"/>
+      <c r="CP292" t="inlineStr"/>
     </row>
     <row r="293">
       <c r="A293" t="n">

</xml_diff>